<commit_message>
changes to descriptions in dataset description file
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t xml:space="preserve">Metadata element</t>
   </si>
@@ -74,13 +74,13 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Descriptive title for the data set. Equivalent to the title of a scientific paper.</t>
+    <t xml:space="preserve">Descriptive title for the data set. Equivalent to the title of a scientific paper. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
   </si>
   <si>
     <t xml:space="preserve">My SPARC dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">Brief description of the study and the data set.  Equivalent to the abstract of a scientific paper.  Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size.</t>
+    <t xml:space="preserve">Brief description of the study and the data set. Equivalent to the abstract of a scientific paper. Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
   </si>
   <si>
     <t xml:space="preserve">A really cool dataset that I collected to answer some question.</t>
@@ -140,6 +140,9 @@
     <t xml:space="preserve">Acknowledgements</t>
   </si>
   <si>
+    <t xml:space="preserve">Acknowledgements beyond funding and contributors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thank you everyone!</t>
   </si>
   <si>
@@ -170,7 +173,7 @@
     <t xml:space="preserve">Additional Links</t>
   </si>
   <si>
-    <t xml:space="preserve">URLs of additional </t>
+    <t xml:space="preserve">URLs of additional resources used by this dataset (e.g., a link to a code repository)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/myuser/code-for-really-cool-data</t>
@@ -200,19 +203,19 @@
     <t xml:space="preserve">Example image filename</t>
   </si>
   <si>
-    <t xml:space="preserve">Name of image file that will be displayed to the public that provides an example of the data</t>
+    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. Name of image file that will be displayed to the public that provides an example of the data</t>
   </si>
   <si>
     <t xml:space="preserve">Example image locator</t>
   </si>
   <si>
-    <t xml:space="preserve">URL or accession number for example image</t>
+    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. URL or accession number for example image</t>
   </si>
   <si>
     <t xml:space="preserve">Example image description</t>
   </si>
   <si>
-    <t xml:space="preserve">Brief caption and figure legend, equivalent to what you would include in a scientific manuscript</t>
+    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. Brief caption and figure legend, equivalent to what you would include in a scientific manuscript</t>
   </si>
   <si>
     <t xml:space="preserve">Completeness of data set</t>
@@ -240,15 +243,19 @@
   </si>
   <si>
     <t xml:space="preserve">Metadata Version DO NOT CHANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -345,10 +352,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -384,7 +391,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,16 +404,20 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -429,7 +440,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,7 +552,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,3191 +577,3193 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="12" t="str">
         <f aca="false">HYPERLINK("https://orcid.org/","ORCID ID. If you don't have an ORCID, we suggest you sign up for one.")</f>
         <v>ORCID ID. If you don't have an ORCID, we suggest you sign up for one.</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="C10" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="C11" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="C12" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>41</v>
       </c>
+      <c r="C14" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>44</v>
       </c>
+      <c r="C15" s="10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="B16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="B17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="B21" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="C21" s="16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="15" t="s">
         <v>60</v>
       </c>
+      <c r="C22" s="16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="B23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C24" s="17" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1.2</v>
+      <c r="A24" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18"/>
+      <c r="B25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18"/>
+      <c r="B27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18"/>
+      <c r="B28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18"/>
+      <c r="B29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="18"/>
+      <c r="B30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18"/>
+      <c r="B31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="18"/>
+      <c r="B32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="18"/>
+      <c r="B33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="18"/>
+      <c r="B34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18"/>
+      <c r="B35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18"/>
+      <c r="B36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="18"/>
+      <c r="B37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="18"/>
+      <c r="B38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="18"/>
+      <c r="B40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18"/>
+      <c r="B41" s="19"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="18"/>
+      <c r="B42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18"/>
+      <c r="B43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="18"/>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="18"/>
+      <c r="B45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="18"/>
+      <c r="B46" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="18"/>
+      <c r="B47" s="19"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="18"/>
+      <c r="B48" s="19"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="18"/>
+      <c r="B49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="18"/>
+      <c r="B50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="18"/>
+      <c r="B51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="18"/>
+      <c r="B52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="18"/>
+      <c r="B53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="18"/>
+      <c r="B54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="18"/>
+      <c r="B55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="18"/>
+      <c r="B56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="18"/>
+      <c r="B57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="18"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="18"/>
+      <c r="B59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="18"/>
+      <c r="B60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="18"/>
+      <c r="B61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="18"/>
+      <c r="B62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="18"/>
+      <c r="B63" s="19"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="18"/>
+      <c r="B64" s="19"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="18"/>
+      <c r="B65" s="19"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="18"/>
+      <c r="B66" s="19"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="18"/>
+      <c r="B67" s="19"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="18"/>
+      <c r="B68" s="19"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="18"/>
+      <c r="B69" s="19"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="18"/>
+      <c r="B70" s="19"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="18"/>
+      <c r="B71" s="19"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="18"/>
+      <c r="B72" s="19"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="18"/>
+      <c r="B73" s="19"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="18"/>
+      <c r="B74" s="19"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="18"/>
+      <c r="B75" s="19"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="18"/>
+      <c r="B76" s="19"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="18"/>
+      <c r="B77" s="19"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="18"/>
+      <c r="B78" s="19"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="18"/>
+      <c r="B79" s="19"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="18"/>
+      <c r="B80" s="19"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="18"/>
+      <c r="B81" s="19"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="18"/>
+      <c r="B82" s="19"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="18"/>
+      <c r="B83" s="19"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="18"/>
+      <c r="B84" s="19"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="18"/>
+      <c r="B85" s="19"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="18"/>
+      <c r="B86" s="19"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="18"/>
+      <c r="B87" s="19"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="18"/>
+      <c r="B88" s="19"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="18"/>
+      <c r="B89" s="19"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="18"/>
+      <c r="B90" s="19"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="18"/>
+      <c r="B91" s="19"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="18"/>
+      <c r="B92" s="19"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="18"/>
+      <c r="B93" s="19"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="18"/>
+      <c r="B94" s="19"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="18"/>
+      <c r="B95" s="19"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="18"/>
+      <c r="B96" s="19"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="18"/>
+      <c r="B97" s="19"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="18"/>
+      <c r="B98" s="19"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="18"/>
+      <c r="B99" s="19"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="18"/>
+      <c r="B100" s="19"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="18"/>
+      <c r="B101" s="19"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="18"/>
+      <c r="B102" s="19"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="18"/>
+      <c r="B103" s="19"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="18"/>
+      <c r="B104" s="19"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="18"/>
+      <c r="B105" s="19"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="18"/>
+      <c r="B106" s="19"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="18"/>
+      <c r="B107" s="19"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="18"/>
+      <c r="B108" s="19"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="18"/>
+      <c r="B109" s="19"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="18"/>
+      <c r="B110" s="19"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="18"/>
+      <c r="B111" s="19"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="18"/>
+      <c r="B112" s="19"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="18"/>
+      <c r="B113" s="19"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="18"/>
+      <c r="B114" s="19"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="18"/>
+      <c r="B115" s="19"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="18"/>
+      <c r="B116" s="19"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="18"/>
+      <c r="B117" s="19"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="18"/>
+      <c r="B118" s="19"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="18"/>
+      <c r="B119" s="19"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="18"/>
+      <c r="B120" s="19"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="18"/>
+      <c r="B121" s="19"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="18"/>
+      <c r="B122" s="19"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="18"/>
+      <c r="B123" s="19"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="18"/>
+      <c r="B124" s="19"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="18"/>
+      <c r="B125" s="19"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="18"/>
+      <c r="B126" s="19"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="18"/>
+      <c r="B127" s="19"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="18"/>
+      <c r="B128" s="19"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="18"/>
+      <c r="B129" s="19"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="18"/>
+      <c r="B130" s="19"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="18"/>
+      <c r="B131" s="19"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="18"/>
+      <c r="B132" s="19"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="18"/>
+      <c r="B133" s="19"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="18"/>
+      <c r="B134" s="19"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="18"/>
+      <c r="B135" s="19"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="18"/>
+      <c r="B136" s="19"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="18"/>
+      <c r="B137" s="19"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="18"/>
+      <c r="B138" s="19"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="18"/>
+      <c r="B139" s="19"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="18"/>
+      <c r="B140" s="19"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="18"/>
+      <c r="B141" s="19"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="18"/>
+      <c r="B142" s="19"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="18"/>
+      <c r="B143" s="19"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="18"/>
+      <c r="B144" s="19"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="18"/>
+      <c r="B145" s="19"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="18"/>
+      <c r="B146" s="19"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="18"/>
+      <c r="B147" s="19"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="18"/>
+      <c r="B148" s="19"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="18"/>
+      <c r="B149" s="19"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="18"/>
+      <c r="B150" s="19"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="18"/>
+      <c r="B151" s="19"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="18"/>
+      <c r="B152" s="19"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="18"/>
+      <c r="B153" s="19"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="18"/>
+      <c r="B154" s="19"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="18"/>
+      <c r="B155" s="19"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="18"/>
+      <c r="B156" s="19"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="18"/>
+      <c r="B157" s="19"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="18"/>
+      <c r="B158" s="19"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="18"/>
+      <c r="B159" s="19"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="18"/>
+      <c r="B160" s="19"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="18"/>
+      <c r="B161" s="19"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="18"/>
+      <c r="B162" s="19"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="18"/>
+      <c r="B163" s="19"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="18"/>
+      <c r="B164" s="19"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="18"/>
+      <c r="B165" s="19"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="18"/>
+      <c r="B166" s="19"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="18"/>
+      <c r="B167" s="19"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="18"/>
+      <c r="B168" s="19"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="18"/>
+      <c r="B169" s="19"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="18"/>
+      <c r="B170" s="19"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="18"/>
+      <c r="B171" s="19"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="18"/>
+      <c r="B172" s="19"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="18"/>
+      <c r="B173" s="19"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="18"/>
+      <c r="B174" s="19"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="18"/>
+      <c r="B175" s="19"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="18"/>
+      <c r="B176" s="19"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="18"/>
+      <c r="B177" s="19"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="18"/>
+      <c r="B178" s="19"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="18"/>
+      <c r="B179" s="19"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="18"/>
+      <c r="B180" s="19"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="18"/>
+      <c r="B181" s="19"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="18"/>
+      <c r="B182" s="19"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="18"/>
+      <c r="B183" s="19"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="18"/>
+      <c r="B184" s="19"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="18"/>
+      <c r="B185" s="19"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="18"/>
+      <c r="B186" s="19"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="18"/>
+      <c r="B187" s="19"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="18"/>
+      <c r="B188" s="19"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="18"/>
+      <c r="B189" s="19"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="18"/>
+      <c r="B190" s="19"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="18"/>
+      <c r="B191" s="19"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="18"/>
+      <c r="B192" s="19"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="18"/>
+      <c r="B193" s="19"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="18"/>
+      <c r="B194" s="19"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="18"/>
+      <c r="B195" s="19"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="18"/>
+      <c r="B196" s="19"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="18"/>
+      <c r="B197" s="19"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="18"/>
+      <c r="B198" s="19"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="18"/>
+      <c r="B199" s="19"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="18"/>
+      <c r="B200" s="19"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="18"/>
+      <c r="B201" s="19"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="18"/>
+      <c r="B202" s="19"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="18"/>
+      <c r="B203" s="19"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="18"/>
+      <c r="B204" s="19"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="18"/>
+      <c r="B205" s="19"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="18"/>
+      <c r="B206" s="19"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="18"/>
+      <c r="B207" s="19"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="18"/>
+      <c r="B208" s="19"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="18"/>
+      <c r="B209" s="19"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="18"/>
+      <c r="B210" s="19"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="18"/>
+      <c r="B211" s="19"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="18"/>
+      <c r="B212" s="19"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="18"/>
+      <c r="B213" s="19"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="18"/>
+      <c r="B214" s="19"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="18"/>
+      <c r="B215" s="19"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="18"/>
+      <c r="B216" s="19"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="18"/>
+      <c r="B217" s="19"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="18"/>
+      <c r="B218" s="19"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="18"/>
+      <c r="B219" s="19"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="18"/>
+      <c r="B220" s="19"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="18"/>
+      <c r="B221" s="19"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="18"/>
+      <c r="B222" s="19"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="18"/>
+      <c r="B223" s="19"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="18"/>
+      <c r="B224" s="19"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="18"/>
+      <c r="B225" s="19"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="18"/>
+      <c r="B226" s="19"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="18"/>
+      <c r="B227" s="19"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="18"/>
+      <c r="B228" s="19"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="18"/>
+      <c r="B229" s="19"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="18"/>
+      <c r="B230" s="19"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="18"/>
+      <c r="B231" s="19"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="18"/>
+      <c r="B232" s="19"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="18"/>
+      <c r="B233" s="19"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="18"/>
+      <c r="B234" s="19"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="18"/>
+      <c r="B235" s="19"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="18"/>
+      <c r="B236" s="19"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="18"/>
+      <c r="B237" s="19"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="18"/>
+      <c r="B238" s="19"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="18"/>
+      <c r="B239" s="19"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="18"/>
+      <c r="B240" s="19"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="18"/>
+      <c r="B241" s="19"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="18"/>
+      <c r="B242" s="19"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="18"/>
+      <c r="B243" s="19"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="18"/>
+      <c r="B244" s="19"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="18"/>
+      <c r="B245" s="19"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="18"/>
+      <c r="B246" s="19"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="18"/>
+      <c r="B247" s="19"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="18"/>
+      <c r="B248" s="19"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="18"/>
+      <c r="B249" s="19"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="18"/>
+      <c r="B250" s="19"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="18"/>
+      <c r="B251" s="19"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="18"/>
+      <c r="B252" s="19"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="18"/>
+      <c r="B253" s="19"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="18"/>
+      <c r="B254" s="19"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="18"/>
+      <c r="B255" s="19"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="18"/>
+      <c r="B256" s="19"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="18"/>
+      <c r="B257" s="19"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="18"/>
+      <c r="B258" s="19"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="18"/>
+      <c r="B259" s="19"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="18"/>
+      <c r="B260" s="19"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="18"/>
+      <c r="B261" s="19"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="18"/>
+      <c r="B262" s="19"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="18"/>
+      <c r="B263" s="19"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="18"/>
+      <c r="B264" s="19"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="18"/>
+      <c r="B265" s="19"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="18"/>
+      <c r="B266" s="19"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="18"/>
+      <c r="B267" s="19"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="18"/>
+      <c r="B268" s="19"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="18"/>
+      <c r="B269" s="19"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="18"/>
+      <c r="B270" s="19"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="18"/>
+      <c r="B271" s="19"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="18"/>
+      <c r="B272" s="19"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="18"/>
+      <c r="B273" s="19"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="18"/>
+      <c r="B274" s="19"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="18"/>
+      <c r="B275" s="19"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="18"/>
+      <c r="B276" s="19"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="18"/>
+      <c r="B277" s="19"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="18"/>
+      <c r="B278" s="19"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="18"/>
+      <c r="B279" s="19"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="18"/>
+      <c r="B280" s="19"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="18"/>
+      <c r="B281" s="19"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="18"/>
+      <c r="B282" s="19"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="18"/>
+      <c r="B283" s="19"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="18"/>
+      <c r="B284" s="19"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="18"/>
+      <c r="B285" s="19"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="18"/>
+      <c r="B286" s="19"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="18"/>
+      <c r="B287" s="19"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="18"/>
+      <c r="B288" s="19"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="18"/>
+      <c r="B289" s="19"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="18"/>
+      <c r="B290" s="19"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="18"/>
+      <c r="B291" s="19"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="18"/>
+      <c r="B292" s="19"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="18"/>
+      <c r="B293" s="19"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="18"/>
+      <c r="B294" s="19"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="18"/>
+      <c r="B295" s="19"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="18"/>
+      <c r="B296" s="19"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="18"/>
+      <c r="B297" s="19"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="18"/>
+      <c r="B298" s="19"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="18"/>
+      <c r="B299" s="19"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="18"/>
+      <c r="B300" s="19"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="18"/>
+      <c r="B301" s="19"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="18"/>
+      <c r="B302" s="19"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="18"/>
+      <c r="B303" s="19"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="18"/>
+      <c r="B304" s="19"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="18"/>
+      <c r="B305" s="19"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="18"/>
+      <c r="B306" s="19"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="18"/>
+      <c r="B307" s="19"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="18"/>
+      <c r="B308" s="19"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="18"/>
+      <c r="B309" s="19"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="18"/>
+      <c r="B310" s="19"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="18"/>
+      <c r="B311" s="19"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B312" s="18"/>
+      <c r="B312" s="19"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B313" s="18"/>
+      <c r="B313" s="19"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B314" s="18"/>
+      <c r="B314" s="19"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B315" s="18"/>
+      <c r="B315" s="19"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B316" s="18"/>
+      <c r="B316" s="19"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B317" s="18"/>
+      <c r="B317" s="19"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B318" s="18"/>
+      <c r="B318" s="19"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B319" s="18"/>
+      <c r="B319" s="19"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B320" s="18"/>
+      <c r="B320" s="19"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B321" s="18"/>
+      <c r="B321" s="19"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B322" s="18"/>
+      <c r="B322" s="19"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B323" s="18"/>
+      <c r="B323" s="19"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B324" s="18"/>
+      <c r="B324" s="19"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B325" s="18"/>
+      <c r="B325" s="19"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B326" s="18"/>
+      <c r="B326" s="19"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B327" s="18"/>
+      <c r="B327" s="19"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B328" s="18"/>
+      <c r="B328" s="19"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B329" s="18"/>
+      <c r="B329" s="19"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B330" s="18"/>
+      <c r="B330" s="19"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B331" s="18"/>
+      <c r="B331" s="19"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="18"/>
+      <c r="B332" s="19"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B333" s="18"/>
+      <c r="B333" s="19"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B334" s="18"/>
+      <c r="B334" s="19"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B335" s="18"/>
+      <c r="B335" s="19"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B336" s="18"/>
+      <c r="B336" s="19"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B337" s="18"/>
+      <c r="B337" s="19"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B338" s="18"/>
+      <c r="B338" s="19"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B339" s="18"/>
+      <c r="B339" s="19"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B340" s="18"/>
+      <c r="B340" s="19"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B341" s="18"/>
+      <c r="B341" s="19"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B342" s="18"/>
+      <c r="B342" s="19"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B343" s="18"/>
+      <c r="B343" s="19"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B344" s="18"/>
+      <c r="B344" s="19"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B345" s="18"/>
+      <c r="B345" s="19"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B346" s="18"/>
+      <c r="B346" s="19"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B347" s="18"/>
+      <c r="B347" s="19"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B348" s="18"/>
+      <c r="B348" s="19"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B349" s="18"/>
+      <c r="B349" s="19"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B350" s="18"/>
+      <c r="B350" s="19"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B351" s="18"/>
+      <c r="B351" s="19"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B352" s="18"/>
+      <c r="B352" s="19"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B353" s="18"/>
+      <c r="B353" s="19"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B354" s="18"/>
+      <c r="B354" s="19"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B355" s="18"/>
+      <c r="B355" s="19"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B356" s="18"/>
+      <c r="B356" s="19"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B357" s="18"/>
+      <c r="B357" s="19"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B358" s="18"/>
+      <c r="B358" s="19"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B359" s="18"/>
+      <c r="B359" s="19"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B360" s="18"/>
+      <c r="B360" s="19"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B361" s="18"/>
+      <c r="B361" s="19"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B362" s="18"/>
+      <c r="B362" s="19"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B363" s="18"/>
+      <c r="B363" s="19"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B364" s="18"/>
+      <c r="B364" s="19"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B365" s="18"/>
+      <c r="B365" s="19"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B366" s="18"/>
+      <c r="B366" s="19"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B367" s="18"/>
+      <c r="B367" s="19"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B368" s="18"/>
+      <c r="B368" s="19"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B369" s="18"/>
+      <c r="B369" s="19"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B370" s="18"/>
+      <c r="B370" s="19"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B371" s="18"/>
+      <c r="B371" s="19"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B372" s="18"/>
+      <c r="B372" s="19"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B373" s="18"/>
+      <c r="B373" s="19"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B374" s="18"/>
+      <c r="B374" s="19"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B375" s="18"/>
+      <c r="B375" s="19"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B376" s="18"/>
+      <c r="B376" s="19"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B377" s="18"/>
+      <c r="B377" s="19"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B378" s="18"/>
+      <c r="B378" s="19"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B379" s="18"/>
+      <c r="B379" s="19"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B380" s="18"/>
+      <c r="B380" s="19"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B381" s="18"/>
+      <c r="B381" s="19"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B382" s="18"/>
+      <c r="B382" s="19"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B383" s="18"/>
+      <c r="B383" s="19"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B384" s="18"/>
+      <c r="B384" s="19"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B385" s="18"/>
+      <c r="B385" s="19"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B386" s="18"/>
+      <c r="B386" s="19"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B387" s="18"/>
+      <c r="B387" s="19"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B388" s="18"/>
+      <c r="B388" s="19"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B389" s="18"/>
+      <c r="B389" s="19"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B390" s="18"/>
+      <c r="B390" s="19"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B391" s="18"/>
+      <c r="B391" s="19"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B392" s="18"/>
+      <c r="B392" s="19"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B393" s="18"/>
+      <c r="B393" s="19"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B394" s="18"/>
+      <c r="B394" s="19"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B395" s="18"/>
+      <c r="B395" s="19"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B396" s="18"/>
+      <c r="B396" s="19"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B397" s="18"/>
+      <c r="B397" s="19"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B398" s="18"/>
+      <c r="B398" s="19"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B399" s="18"/>
+      <c r="B399" s="19"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B400" s="18"/>
+      <c r="B400" s="19"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B401" s="18"/>
+      <c r="B401" s="19"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B402" s="18"/>
+      <c r="B402" s="19"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B403" s="18"/>
+      <c r="B403" s="19"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B404" s="18"/>
+      <c r="B404" s="19"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B405" s="18"/>
+      <c r="B405" s="19"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B406" s="18"/>
+      <c r="B406" s="19"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B407" s="18"/>
+      <c r="B407" s="19"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B408" s="18"/>
+      <c r="B408" s="19"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B409" s="18"/>
+      <c r="B409" s="19"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B410" s="18"/>
+      <c r="B410" s="19"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B411" s="18"/>
+      <c r="B411" s="19"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B412" s="18"/>
+      <c r="B412" s="19"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B413" s="18"/>
+      <c r="B413" s="19"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B414" s="18"/>
+      <c r="B414" s="19"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B415" s="18"/>
+      <c r="B415" s="19"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B416" s="18"/>
+      <c r="B416" s="19"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B417" s="18"/>
+      <c r="B417" s="19"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B418" s="18"/>
+      <c r="B418" s="19"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B419" s="18"/>
+      <c r="B419" s="19"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B420" s="18"/>
+      <c r="B420" s="19"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B421" s="18"/>
+      <c r="B421" s="19"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B422" s="18"/>
+      <c r="B422" s="19"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B423" s="18"/>
+      <c r="B423" s="19"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B424" s="18"/>
+      <c r="B424" s="19"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B425" s="18"/>
+      <c r="B425" s="19"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B426" s="18"/>
+      <c r="B426" s="19"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B427" s="18"/>
+      <c r="B427" s="19"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B428" s="18"/>
+      <c r="B428" s="19"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B429" s="18"/>
+      <c r="B429" s="19"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B430" s="18"/>
+      <c r="B430" s="19"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B431" s="18"/>
+      <c r="B431" s="19"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B432" s="18"/>
+      <c r="B432" s="19"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B433" s="18"/>
+      <c r="B433" s="19"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B434" s="18"/>
+      <c r="B434" s="19"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B435" s="18"/>
+      <c r="B435" s="19"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B436" s="18"/>
+      <c r="B436" s="19"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B437" s="18"/>
+      <c r="B437" s="19"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B438" s="18"/>
+      <c r="B438" s="19"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B439" s="18"/>
+      <c r="B439" s="19"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B440" s="18"/>
+      <c r="B440" s="19"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B441" s="18"/>
+      <c r="B441" s="19"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B442" s="18"/>
+      <c r="B442" s="19"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B443" s="18"/>
+      <c r="B443" s="19"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B444" s="18"/>
+      <c r="B444" s="19"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B445" s="18"/>
+      <c r="B445" s="19"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B446" s="18"/>
+      <c r="B446" s="19"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B447" s="18"/>
+      <c r="B447" s="19"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B448" s="18"/>
+      <c r="B448" s="19"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B449" s="18"/>
+      <c r="B449" s="19"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B450" s="18"/>
+      <c r="B450" s="19"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B451" s="18"/>
+      <c r="B451" s="19"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B452" s="18"/>
+      <c r="B452" s="19"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B453" s="18"/>
+      <c r="B453" s="19"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B454" s="18"/>
+      <c r="B454" s="19"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B455" s="18"/>
+      <c r="B455" s="19"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B456" s="18"/>
+      <c r="B456" s="19"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B457" s="18"/>
+      <c r="B457" s="19"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B458" s="18"/>
+      <c r="B458" s="19"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B459" s="18"/>
+      <c r="B459" s="19"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B460" s="18"/>
+      <c r="B460" s="19"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B461" s="18"/>
+      <c r="B461" s="19"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B462" s="18"/>
+      <c r="B462" s="19"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B463" s="18"/>
+      <c r="B463" s="19"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B464" s="18"/>
+      <c r="B464" s="19"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B465" s="18"/>
+      <c r="B465" s="19"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B466" s="18"/>
+      <c r="B466" s="19"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B467" s="18"/>
+      <c r="B467" s="19"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B468" s="18"/>
+      <c r="B468" s="19"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B469" s="18"/>
+      <c r="B469" s="19"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B470" s="18"/>
+      <c r="B470" s="19"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B471" s="18"/>
+      <c r="B471" s="19"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B472" s="18"/>
+      <c r="B472" s="19"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B473" s="18"/>
+      <c r="B473" s="19"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B474" s="18"/>
+      <c r="B474" s="19"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B475" s="18"/>
+      <c r="B475" s="19"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B476" s="18"/>
+      <c r="B476" s="19"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B477" s="18"/>
+      <c r="B477" s="19"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B478" s="18"/>
+      <c r="B478" s="19"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B479" s="18"/>
+      <c r="B479" s="19"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B480" s="18"/>
+      <c r="B480" s="19"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B481" s="18"/>
+      <c r="B481" s="19"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B482" s="18"/>
+      <c r="B482" s="19"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B483" s="18"/>
+      <c r="B483" s="19"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B484" s="18"/>
+      <c r="B484" s="19"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B485" s="18"/>
+      <c r="B485" s="19"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B486" s="18"/>
+      <c r="B486" s="19"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B487" s="18"/>
+      <c r="B487" s="19"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B488" s="18"/>
+      <c r="B488" s="19"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B489" s="18"/>
+      <c r="B489" s="19"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B490" s="18"/>
+      <c r="B490" s="19"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B491" s="18"/>
+      <c r="B491" s="19"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B492" s="18"/>
+      <c r="B492" s="19"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B493" s="18"/>
+      <c r="B493" s="19"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B494" s="18"/>
+      <c r="B494" s="19"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B495" s="18"/>
+      <c r="B495" s="19"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B496" s="18"/>
+      <c r="B496" s="19"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B497" s="18"/>
+      <c r="B497" s="19"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B498" s="18"/>
+      <c r="B498" s="19"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B499" s="18"/>
+      <c r="B499" s="19"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B500" s="18"/>
+      <c r="B500" s="19"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B501" s="18"/>
+      <c r="B501" s="19"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B502" s="18"/>
+      <c r="B502" s="19"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B503" s="18"/>
+      <c r="B503" s="19"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B504" s="18"/>
+      <c r="B504" s="19"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B505" s="18"/>
+      <c r="B505" s="19"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B506" s="18"/>
+      <c r="B506" s="19"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B507" s="18"/>
+      <c r="B507" s="19"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B508" s="18"/>
+      <c r="B508" s="19"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B509" s="18"/>
+      <c r="B509" s="19"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B510" s="18"/>
+      <c r="B510" s="19"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B511" s="18"/>
+      <c r="B511" s="19"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B512" s="18"/>
+      <c r="B512" s="19"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B513" s="18"/>
+      <c r="B513" s="19"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B514" s="18"/>
+      <c r="B514" s="19"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B515" s="18"/>
+      <c r="B515" s="19"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B516" s="18"/>
+      <c r="B516" s="19"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B517" s="18"/>
+      <c r="B517" s="19"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B518" s="18"/>
+      <c r="B518" s="19"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B519" s="18"/>
+      <c r="B519" s="19"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B520" s="18"/>
+      <c r="B520" s="19"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B521" s="18"/>
+      <c r="B521" s="19"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B522" s="18"/>
+      <c r="B522" s="19"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B523" s="18"/>
+      <c r="B523" s="19"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B524" s="18"/>
+      <c r="B524" s="19"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B525" s="18"/>
+      <c r="B525" s="19"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B526" s="18"/>
+      <c r="B526" s="19"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B527" s="18"/>
+      <c r="B527" s="19"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B528" s="18"/>
+      <c r="B528" s="19"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B529" s="18"/>
+      <c r="B529" s="19"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B530" s="18"/>
+      <c r="B530" s="19"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B531" s="18"/>
+      <c r="B531" s="19"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B532" s="18"/>
+      <c r="B532" s="19"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B533" s="18"/>
+      <c r="B533" s="19"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B534" s="18"/>
+      <c r="B534" s="19"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B535" s="18"/>
+      <c r="B535" s="19"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B536" s="18"/>
+      <c r="B536" s="19"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B537" s="18"/>
+      <c r="B537" s="19"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B538" s="18"/>
+      <c r="B538" s="19"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B539" s="18"/>
+      <c r="B539" s="19"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B540" s="18"/>
+      <c r="B540" s="19"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B541" s="18"/>
+      <c r="B541" s="19"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B542" s="18"/>
+      <c r="B542" s="19"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B543" s="18"/>
+      <c r="B543" s="19"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B544" s="18"/>
+      <c r="B544" s="19"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B545" s="18"/>
+      <c r="B545" s="19"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B546" s="18"/>
+      <c r="B546" s="19"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B547" s="18"/>
+      <c r="B547" s="19"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B548" s="18"/>
+      <c r="B548" s="19"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B549" s="18"/>
+      <c r="B549" s="19"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B550" s="18"/>
+      <c r="B550" s="19"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B551" s="18"/>
+      <c r="B551" s="19"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B552" s="18"/>
+      <c r="B552" s="19"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B553" s="18"/>
+      <c r="B553" s="19"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B554" s="18"/>
+      <c r="B554" s="19"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B555" s="18"/>
+      <c r="B555" s="19"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B556" s="18"/>
+      <c r="B556" s="19"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B557" s="18"/>
+      <c r="B557" s="19"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B558" s="18"/>
+      <c r="B558" s="19"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B559" s="18"/>
+      <c r="B559" s="19"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B560" s="18"/>
+      <c r="B560" s="19"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B561" s="18"/>
+      <c r="B561" s="19"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B562" s="18"/>
+      <c r="B562" s="19"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B563" s="18"/>
+      <c r="B563" s="19"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B564" s="18"/>
+      <c r="B564" s="19"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B565" s="18"/>
+      <c r="B565" s="19"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B566" s="18"/>
+      <c r="B566" s="19"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B567" s="18"/>
+      <c r="B567" s="19"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B568" s="18"/>
+      <c r="B568" s="19"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B569" s="18"/>
+      <c r="B569" s="19"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B570" s="18"/>
+      <c r="B570" s="19"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B571" s="18"/>
+      <c r="B571" s="19"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B572" s="18"/>
+      <c r="B572" s="19"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B573" s="18"/>
+      <c r="B573" s="19"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B574" s="18"/>
+      <c r="B574" s="19"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B575" s="18"/>
+      <c r="B575" s="19"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B576" s="18"/>
+      <c r="B576" s="19"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B577" s="18"/>
+      <c r="B577" s="19"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B578" s="18"/>
+      <c r="B578" s="19"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B579" s="18"/>
+      <c r="B579" s="19"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B580" s="18"/>
+      <c r="B580" s="19"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B581" s="18"/>
+      <c r="B581" s="19"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B582" s="18"/>
+      <c r="B582" s="19"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B583" s="18"/>
+      <c r="B583" s="19"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B584" s="18"/>
+      <c r="B584" s="19"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B585" s="18"/>
+      <c r="B585" s="19"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B586" s="18"/>
+      <c r="B586" s="19"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B587" s="18"/>
+      <c r="B587" s="19"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B588" s="18"/>
+      <c r="B588" s="19"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B589" s="18"/>
+      <c r="B589" s="19"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B590" s="18"/>
+      <c r="B590" s="19"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B591" s="18"/>
+      <c r="B591" s="19"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B592" s="18"/>
+      <c r="B592" s="19"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B593" s="18"/>
+      <c r="B593" s="19"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B594" s="18"/>
+      <c r="B594" s="19"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B595" s="18"/>
+      <c r="B595" s="19"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B596" s="18"/>
+      <c r="B596" s="19"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B597" s="18"/>
+      <c r="B597" s="19"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B598" s="18"/>
+      <c r="B598" s="19"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B599" s="18"/>
+      <c r="B599" s="19"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B600" s="18"/>
+      <c r="B600" s="19"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B601" s="18"/>
+      <c r="B601" s="19"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B602" s="18"/>
+      <c r="B602" s="19"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B603" s="18"/>
+      <c r="B603" s="19"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B604" s="18"/>
+      <c r="B604" s="19"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B605" s="18"/>
+      <c r="B605" s="19"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B606" s="18"/>
+      <c r="B606" s="19"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B607" s="18"/>
+      <c r="B607" s="19"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B608" s="18"/>
+      <c r="B608" s="19"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B609" s="18"/>
+      <c r="B609" s="19"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B610" s="18"/>
+      <c r="B610" s="19"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B611" s="18"/>
+      <c r="B611" s="19"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B612" s="18"/>
+      <c r="B612" s="19"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B613" s="18"/>
+      <c r="B613" s="19"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B614" s="18"/>
+      <c r="B614" s="19"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B615" s="18"/>
+      <c r="B615" s="19"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B616" s="18"/>
+      <c r="B616" s="19"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B617" s="18"/>
+      <c r="B617" s="19"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B618" s="18"/>
+      <c r="B618" s="19"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B619" s="18"/>
+      <c r="B619" s="19"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B620" s="18"/>
+      <c r="B620" s="19"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B621" s="18"/>
+      <c r="B621" s="19"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B622" s="18"/>
+      <c r="B622" s="19"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B623" s="18"/>
+      <c r="B623" s="19"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B624" s="18"/>
+      <c r="B624" s="19"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B625" s="18"/>
+      <c r="B625" s="19"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B626" s="18"/>
+      <c r="B626" s="19"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B627" s="18"/>
+      <c r="B627" s="19"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B628" s="18"/>
+      <c r="B628" s="19"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B629" s="18"/>
+      <c r="B629" s="19"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B630" s="18"/>
+      <c r="B630" s="19"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B631" s="18"/>
+      <c r="B631" s="19"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B632" s="18"/>
+      <c r="B632" s="19"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B633" s="18"/>
+      <c r="B633" s="19"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B634" s="18"/>
+      <c r="B634" s="19"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B635" s="18"/>
+      <c r="B635" s="19"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B636" s="18"/>
+      <c r="B636" s="19"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B637" s="18"/>
+      <c r="B637" s="19"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B638" s="18"/>
+      <c r="B638" s="19"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B639" s="18"/>
+      <c r="B639" s="19"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B640" s="18"/>
+      <c r="B640" s="19"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B641" s="18"/>
+      <c r="B641" s="19"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B642" s="18"/>
+      <c r="B642" s="19"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B643" s="18"/>
+      <c r="B643" s="19"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B644" s="18"/>
+      <c r="B644" s="19"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B645" s="18"/>
+      <c r="B645" s="19"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B646" s="18"/>
+      <c r="B646" s="19"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B647" s="18"/>
+      <c r="B647" s="19"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B648" s="18"/>
+      <c r="B648" s="19"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B649" s="18"/>
+      <c r="B649" s="19"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B650" s="18"/>
+      <c r="B650" s="19"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B651" s="18"/>
+      <c r="B651" s="19"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B652" s="18"/>
+      <c r="B652" s="19"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B653" s="18"/>
+      <c r="B653" s="19"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B654" s="18"/>
+      <c r="B654" s="19"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B655" s="18"/>
+      <c r="B655" s="19"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B656" s="18"/>
+      <c r="B656" s="19"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B657" s="18"/>
+      <c r="B657" s="19"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B658" s="18"/>
+      <c r="B658" s="19"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B659" s="18"/>
+      <c r="B659" s="19"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B660" s="18"/>
+      <c r="B660" s="19"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B661" s="18"/>
+      <c r="B661" s="19"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B662" s="18"/>
+      <c r="B662" s="19"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B663" s="18"/>
+      <c r="B663" s="19"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B664" s="18"/>
+      <c r="B664" s="19"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B665" s="18"/>
+      <c r="B665" s="19"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B666" s="18"/>
+      <c r="B666" s="19"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B667" s="18"/>
+      <c r="B667" s="19"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B668" s="18"/>
+      <c r="B668" s="19"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B669" s="18"/>
+      <c r="B669" s="19"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B670" s="18"/>
+      <c r="B670" s="19"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B671" s="18"/>
+      <c r="B671" s="19"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B672" s="18"/>
+      <c r="B672" s="19"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B673" s="18"/>
+      <c r="B673" s="19"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B674" s="18"/>
+      <c r="B674" s="19"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B675" s="18"/>
+      <c r="B675" s="19"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B676" s="18"/>
+      <c r="B676" s="19"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B677" s="18"/>
+      <c r="B677" s="19"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B678" s="18"/>
+      <c r="B678" s="19"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B679" s="18"/>
+      <c r="B679" s="19"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B680" s="18"/>
+      <c r="B680" s="19"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B681" s="18"/>
+      <c r="B681" s="19"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B682" s="18"/>
+      <c r="B682" s="19"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B683" s="18"/>
+      <c r="B683" s="19"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B684" s="18"/>
+      <c r="B684" s="19"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B685" s="18"/>
+      <c r="B685" s="19"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B686" s="18"/>
+      <c r="B686" s="19"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B687" s="18"/>
+      <c r="B687" s="19"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B688" s="18"/>
+      <c r="B688" s="19"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B689" s="18"/>
+      <c r="B689" s="19"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B690" s="18"/>
+      <c r="B690" s="19"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B691" s="18"/>
+      <c r="B691" s="19"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B692" s="18"/>
+      <c r="B692" s="19"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B693" s="18"/>
+      <c r="B693" s="19"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B694" s="18"/>
+      <c r="B694" s="19"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B695" s="18"/>
+      <c r="B695" s="19"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B696" s="18"/>
+      <c r="B696" s="19"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B697" s="18"/>
+      <c r="B697" s="19"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B698" s="18"/>
+      <c r="B698" s="19"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B699" s="18"/>
+      <c r="B699" s="19"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B700" s="18"/>
+      <c r="B700" s="19"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B701" s="18"/>
+      <c r="B701" s="19"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B702" s="18"/>
+      <c r="B702" s="19"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B703" s="18"/>
+      <c r="B703" s="19"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B704" s="18"/>
+      <c r="B704" s="19"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B705" s="18"/>
+      <c r="B705" s="19"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B706" s="18"/>
+      <c r="B706" s="19"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B707" s="18"/>
+      <c r="B707" s="19"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B708" s="18"/>
+      <c r="B708" s="19"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B709" s="18"/>
+      <c r="B709" s="19"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B710" s="18"/>
+      <c r="B710" s="19"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B711" s="18"/>
+      <c r="B711" s="19"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B712" s="18"/>
+      <c r="B712" s="19"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B713" s="18"/>
+      <c r="B713" s="19"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B714" s="18"/>
+      <c r="B714" s="19"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B715" s="18"/>
+      <c r="B715" s="19"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B716" s="18"/>
+      <c r="B716" s="19"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B717" s="18"/>
+      <c r="B717" s="19"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B718" s="18"/>
+      <c r="B718" s="19"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B719" s="18"/>
+      <c r="B719" s="19"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B720" s="18"/>
+      <c r="B720" s="19"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B721" s="18"/>
+      <c r="B721" s="19"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B722" s="18"/>
+      <c r="B722" s="19"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B723" s="18"/>
+      <c r="B723" s="19"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B724" s="18"/>
+      <c r="B724" s="19"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B725" s="18"/>
+      <c r="B725" s="19"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B726" s="18"/>
+      <c r="B726" s="19"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B727" s="18"/>
+      <c r="B727" s="19"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B728" s="18"/>
+      <c r="B728" s="19"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B729" s="18"/>
+      <c r="B729" s="19"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B730" s="18"/>
+      <c r="B730" s="19"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B731" s="18"/>
+      <c r="B731" s="19"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B732" s="18"/>
+      <c r="B732" s="19"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B733" s="18"/>
+      <c r="B733" s="19"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B734" s="18"/>
+      <c r="B734" s="19"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B735" s="18"/>
+      <c r="B735" s="19"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B736" s="18"/>
+      <c r="B736" s="19"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B737" s="18"/>
+      <c r="B737" s="19"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B738" s="18"/>
+      <c r="B738" s="19"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B739" s="18"/>
+      <c r="B739" s="19"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B740" s="18"/>
+      <c r="B740" s="19"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B741" s="18"/>
+      <c r="B741" s="19"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B742" s="18"/>
+      <c r="B742" s="19"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B743" s="18"/>
+      <c r="B743" s="19"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B744" s="18"/>
+      <c r="B744" s="19"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B745" s="18"/>
+      <c r="B745" s="19"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B746" s="18"/>
+      <c r="B746" s="19"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B747" s="18"/>
+      <c r="B747" s="19"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B748" s="18"/>
+      <c r="B748" s="19"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B749" s="18"/>
+      <c r="B749" s="19"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B750" s="18"/>
+      <c r="B750" s="19"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B751" s="18"/>
+      <c r="B751" s="19"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B752" s="18"/>
+      <c r="B752" s="19"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B753" s="18"/>
+      <c r="B753" s="19"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B754" s="18"/>
+      <c r="B754" s="19"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B755" s="18"/>
+      <c r="B755" s="19"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B756" s="18"/>
+      <c r="B756" s="19"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B757" s="18"/>
+      <c r="B757" s="19"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B758" s="18"/>
+      <c r="B758" s="19"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B759" s="18"/>
+      <c r="B759" s="19"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B760" s="18"/>
+      <c r="B760" s="19"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B761" s="18"/>
+      <c r="B761" s="19"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B762" s="18"/>
+      <c r="B762" s="19"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B763" s="18"/>
+      <c r="B763" s="19"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B764" s="18"/>
+      <c r="B764" s="19"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B765" s="18"/>
+      <c r="B765" s="19"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B766" s="18"/>
+      <c r="B766" s="19"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B767" s="18"/>
+      <c r="B767" s="19"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B768" s="18"/>
+      <c r="B768" s="19"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B769" s="18"/>
+      <c r="B769" s="19"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B770" s="18"/>
+      <c r="B770" s="19"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B771" s="18"/>
+      <c r="B771" s="19"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B772" s="18"/>
+      <c r="B772" s="19"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B773" s="18"/>
+      <c r="B773" s="19"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B774" s="18"/>
+      <c r="B774" s="19"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B775" s="18"/>
+      <c r="B775" s="19"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B776" s="18"/>
+      <c r="B776" s="19"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B777" s="18"/>
+      <c r="B777" s="19"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B778" s="18"/>
+      <c r="B778" s="19"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B779" s="18"/>
+      <c r="B779" s="19"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B780" s="18"/>
+      <c r="B780" s="19"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B781" s="18"/>
+      <c r="B781" s="19"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B782" s="18"/>
+      <c r="B782" s="19"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B783" s="18"/>
+      <c r="B783" s="19"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B784" s="18"/>
+      <c r="B784" s="19"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B785" s="18"/>
+      <c r="B785" s="19"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B786" s="18"/>
+      <c r="B786" s="19"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B787" s="18"/>
+      <c r="B787" s="19"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B788" s="18"/>
+      <c r="B788" s="19"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B789" s="18"/>
+      <c r="B789" s="19"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B790" s="18"/>
+      <c r="B790" s="19"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B791" s="18"/>
+      <c r="B791" s="19"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B792" s="18"/>
+      <c r="B792" s="19"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B793" s="18"/>
+      <c r="B793" s="19"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B794" s="18"/>
+      <c r="B794" s="19"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B795" s="18"/>
+      <c r="B795" s="19"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B796" s="18"/>
+      <c r="B796" s="19"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B797" s="18"/>
+      <c r="B797" s="19"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B798" s="18"/>
+      <c r="B798" s="19"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B799" s="18"/>
+      <c r="B799" s="19"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B800" s="18"/>
+      <c r="B800" s="19"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B801" s="18"/>
+      <c r="B801" s="19"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B802" s="18"/>
+      <c r="B802" s="19"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B803" s="18"/>
+      <c r="B803" s="19"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B804" s="18"/>
+      <c r="B804" s="19"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B805" s="18"/>
+      <c r="B805" s="19"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B806" s="18"/>
+      <c r="B806" s="19"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B807" s="18"/>
+      <c r="B807" s="19"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B808" s="18"/>
+      <c r="B808" s="19"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B809" s="18"/>
+      <c r="B809" s="19"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B810" s="18"/>
+      <c r="B810" s="19"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B811" s="18"/>
+      <c r="B811" s="19"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B812" s="18"/>
+      <c r="B812" s="19"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B813" s="18"/>
+      <c r="B813" s="19"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B814" s="18"/>
+      <c r="B814" s="19"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B815" s="18"/>
+      <c r="B815" s="19"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B816" s="18"/>
+      <c r="B816" s="19"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B817" s="18"/>
+      <c r="B817" s="19"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B818" s="18"/>
+      <c r="B818" s="19"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B819" s="18"/>
+      <c r="B819" s="19"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B820" s="18"/>
+      <c r="B820" s="19"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B821" s="18"/>
+      <c r="B821" s="19"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B822" s="18"/>
+      <c r="B822" s="19"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B823" s="18"/>
+      <c r="B823" s="19"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B824" s="18"/>
+      <c r="B824" s="19"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B825" s="18"/>
+      <c r="B825" s="19"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B826" s="18"/>
+      <c r="B826" s="19"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B827" s="18"/>
+      <c r="B827" s="19"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B828" s="18"/>
+      <c r="B828" s="19"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B829" s="18"/>
+      <c r="B829" s="19"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B830" s="18"/>
+      <c r="B830" s="19"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B831" s="18"/>
+      <c r="B831" s="19"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B832" s="18"/>
+      <c r="B832" s="19"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B833" s="18"/>
+      <c r="B833" s="19"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B834" s="18"/>
+      <c r="B834" s="19"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B835" s="18"/>
+      <c r="B835" s="19"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B836" s="18"/>
+      <c r="B836" s="19"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B837" s="18"/>
+      <c r="B837" s="19"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B838" s="18"/>
+      <c r="B838" s="19"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B839" s="18"/>
+      <c r="B839" s="19"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B840" s="18"/>
+      <c r="B840" s="19"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B841" s="18"/>
+      <c r="B841" s="19"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B842" s="18"/>
+      <c r="B842" s="19"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B843" s="18"/>
+      <c r="B843" s="19"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B844" s="18"/>
+      <c r="B844" s="19"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B845" s="18"/>
+      <c r="B845" s="19"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B846" s="18"/>
+      <c r="B846" s="19"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B847" s="18"/>
+      <c r="B847" s="19"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B848" s="18"/>
+      <c r="B848" s="19"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B849" s="18"/>
+      <c r="B849" s="19"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B850" s="18"/>
+      <c r="B850" s="19"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B851" s="18"/>
+      <c r="B851" s="19"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B852" s="18"/>
+      <c r="B852" s="19"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B853" s="18"/>
+      <c r="B853" s="19"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B854" s="18"/>
+      <c r="B854" s="19"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B855" s="18"/>
+      <c r="B855" s="19"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B856" s="18"/>
+      <c r="B856" s="19"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B857" s="18"/>
+      <c r="B857" s="19"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B858" s="18"/>
+      <c r="B858" s="19"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B859" s="18"/>
+      <c r="B859" s="19"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B860" s="18"/>
+      <c r="B860" s="19"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B861" s="18"/>
+      <c r="B861" s="19"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B862" s="18"/>
+      <c r="B862" s="19"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B863" s="18"/>
+      <c r="B863" s="19"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B864" s="18"/>
+      <c r="B864" s="19"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B865" s="18"/>
+      <c r="B865" s="19"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B866" s="18"/>
+      <c r="B866" s="19"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B867" s="18"/>
+      <c r="B867" s="19"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B868" s="18"/>
+      <c r="B868" s="19"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B869" s="18"/>
+      <c r="B869" s="19"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B870" s="18"/>
+      <c r="B870" s="19"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B871" s="18"/>
+      <c r="B871" s="19"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B872" s="18"/>
+      <c r="B872" s="19"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B873" s="18"/>
+      <c r="B873" s="19"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B874" s="18"/>
+      <c r="B874" s="19"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B875" s="18"/>
+      <c r="B875" s="19"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B876" s="18"/>
+      <c r="B876" s="19"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B877" s="18"/>
+      <c r="B877" s="19"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B878" s="18"/>
+      <c r="B878" s="19"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B879" s="18"/>
+      <c r="B879" s="19"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B880" s="18"/>
+      <c r="B880" s="19"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B881" s="18"/>
+      <c r="B881" s="19"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B882" s="18"/>
+      <c r="B882" s="19"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B883" s="18"/>
+      <c r="B883" s="19"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B884" s="18"/>
+      <c r="B884" s="19"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B885" s="18"/>
+      <c r="B885" s="19"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B886" s="18"/>
+      <c r="B886" s="19"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B887" s="18"/>
+      <c r="B887" s="19"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B888" s="18"/>
+      <c r="B888" s="19"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B889" s="18"/>
+      <c r="B889" s="19"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B890" s="18"/>
+      <c r="B890" s="19"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B891" s="18"/>
+      <c r="B891" s="19"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B892" s="18"/>
+      <c r="B892" s="19"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B893" s="18"/>
+      <c r="B893" s="19"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B894" s="18"/>
+      <c r="B894" s="19"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B895" s="18"/>
+      <c r="B895" s="19"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B896" s="18"/>
+      <c r="B896" s="19"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B897" s="18"/>
+      <c r="B897" s="19"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B898" s="18"/>
+      <c r="B898" s="19"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B899" s="18"/>
+      <c r="B899" s="19"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B900" s="18"/>
+      <c r="B900" s="19"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B901" s="18"/>
+      <c r="B901" s="19"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B902" s="18"/>
+      <c r="B902" s="19"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B903" s="18"/>
+      <c r="B903" s="19"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B904" s="18"/>
+      <c r="B904" s="19"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B905" s="18"/>
+      <c r="B905" s="19"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B906" s="18"/>
+      <c r="B906" s="19"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B907" s="18"/>
+      <c r="B907" s="19"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B908" s="18"/>
+      <c r="B908" s="19"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B909" s="18"/>
+      <c r="B909" s="19"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B910" s="18"/>
+      <c r="B910" s="19"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B911" s="18"/>
+      <c r="B911" s="19"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B912" s="18"/>
+      <c r="B912" s="19"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B913" s="18"/>
+      <c r="B913" s="19"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B914" s="18"/>
+      <c r="B914" s="19"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B915" s="18"/>
+      <c r="B915" s="19"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B916" s="18"/>
+      <c r="B916" s="19"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B917" s="18"/>
+      <c r="B917" s="19"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B918" s="18"/>
+      <c r="B918" s="19"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B919" s="18"/>
+      <c r="B919" s="19"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B920" s="18"/>
+      <c r="B920" s="19"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B921" s="18"/>
+      <c r="B921" s="19"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B922" s="18"/>
+      <c r="B922" s="19"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B923" s="18"/>
+      <c r="B923" s="19"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B924" s="18"/>
+      <c r="B924" s="19"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B925" s="18"/>
+      <c r="B925" s="19"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B926" s="18"/>
+      <c r="B926" s="19"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B927" s="18"/>
+      <c r="B927" s="19"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B928" s="18"/>
+      <c r="B928" s="19"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B929" s="18"/>
+      <c r="B929" s="19"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B930" s="18"/>
+      <c r="B930" s="19"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B931" s="18"/>
+      <c r="B931" s="19"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B932" s="18"/>
+      <c r="B932" s="19"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B933" s="18"/>
+      <c r="B933" s="19"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B934" s="18"/>
+      <c r="B934" s="19"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B935" s="18"/>
+      <c r="B935" s="19"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B936" s="18"/>
+      <c r="B936" s="19"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B937" s="18"/>
+      <c r="B937" s="19"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B938" s="18"/>
+      <c r="B938" s="19"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B939" s="18"/>
+      <c r="B939" s="19"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B940" s="18"/>
+      <c r="B940" s="19"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B941" s="18"/>
+      <c r="B941" s="19"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B942" s="18"/>
+      <c r="B942" s="19"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B943" s="18"/>
+      <c r="B943" s="19"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B944" s="18"/>
+      <c r="B944" s="19"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B945" s="18"/>
+      <c r="B945" s="19"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B946" s="18"/>
+      <c r="B946" s="19"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B947" s="18"/>
+      <c r="B947" s="19"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B948" s="18"/>
+      <c r="B948" s="19"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B949" s="18"/>
+      <c r="B949" s="19"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B950" s="18"/>
+      <c r="B950" s="19"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B951" s="18"/>
+      <c r="B951" s="19"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B952" s="18"/>
+      <c r="B952" s="19"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B953" s="18"/>
+      <c r="B953" s="19"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B954" s="18"/>
+      <c r="B954" s="19"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B955" s="18"/>
+      <c r="B955" s="19"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B956" s="18"/>
+      <c r="B956" s="19"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B957" s="18"/>
+      <c r="B957" s="19"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B958" s="18"/>
+      <c r="B958" s="19"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B959" s="18"/>
+      <c r="B959" s="19"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B960" s="18"/>
+      <c r="B960" s="19"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B961" s="18"/>
+      <c r="B961" s="19"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B962" s="18"/>
+      <c r="B962" s="19"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B963" s="18"/>
+      <c r="B963" s="19"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B964" s="18"/>
+      <c r="B964" s="19"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B965" s="18"/>
+      <c r="B965" s="19"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B966" s="18"/>
+      <c r="B966" s="19"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B967" s="18"/>
+      <c r="B967" s="19"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B968" s="18"/>
+      <c r="B968" s="19"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B969" s="18"/>
+      <c r="B969" s="19"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B970" s="18"/>
+      <c r="B970" s="19"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B971" s="18"/>
+      <c r="B971" s="19"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B972" s="18"/>
+      <c r="B972" s="19"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B973" s="18"/>
+      <c r="B973" s="19"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B974" s="18"/>
+      <c r="B974" s="19"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B975" s="18"/>
+      <c r="B975" s="19"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B976" s="18"/>
+      <c r="B976" s="19"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B977" s="18"/>
+      <c r="B977" s="19"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B978" s="18"/>
+      <c r="B978" s="19"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B979" s="18"/>
+      <c r="B979" s="19"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B980" s="18"/>
+      <c r="B980" s="19"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B981" s="18"/>
+      <c r="B981" s="19"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B982" s="18"/>
+      <c r="B982" s="19"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B983" s="18"/>
+      <c r="B983" s="19"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B984" s="18"/>
+      <c r="B984" s="19"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B985" s="18"/>
+      <c r="B985" s="19"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B986" s="18"/>
+      <c r="B986" s="19"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B987" s="18"/>
+      <c r="B987" s="19"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B988" s="18"/>
+      <c r="B988" s="19"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B989" s="18"/>
+      <c r="B989" s="19"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B990" s="18"/>
+      <c r="B990" s="19"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B991" s="18"/>
+      <c r="B991" s="19"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B992" s="18"/>
+      <c r="B992" s="19"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B993" s="18"/>
+      <c r="B993" s="19"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B994" s="18"/>
+      <c r="B994" s="19"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B995" s="18"/>
+      <c r="B995" s="19"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B996" s="18"/>
+      <c r="B996" s="19"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B997" s="18"/>
+      <c r="B997" s="19"/>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B998" s="18"/>
+      <c r="B998" s="19"/>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B999" s="18"/>
+      <c r="B999" s="19"/>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1000" s="18"/>
+      <c r="B1000" s="19"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
dataset description remove example image fields
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t xml:space="preserve">Metadata element</t>
   </si>
@@ -198,24 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of unique samples in this dataset, should match samples metadata file. Set to zero if there are no samples.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example image filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. Name of image file that will be displayed to the public that provides an example of the data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example image locator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. URL or accession number for example image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example image description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independent of this field, please add the banner image to the dataset on Blackfynn. Brief caption and figure legend, equivalent to what you would include in a scientific manuscript</t>
   </si>
   <si>
     <t xml:space="preserve">Completeness of data set</t>
@@ -552,7 +534,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,70 +754,52 @@
       <c r="B18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="16" t="s">
         <v>58</v>
       </c>
+      <c r="B21" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="B22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="16"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="19"/>
@@ -3756,15 +3720,9 @@
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B997" s="19"/>
     </row>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B998" s="19"/>
-    </row>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B999" s="19"/>
-    </row>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1000" s="19"/>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
dataset description update desc and originating descriptions
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -80,7 +80,7 @@
     <t xml:space="preserve">My SPARC dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">Brief description of the study and the data set. Equivalent to the abstract of a scientific paper. Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
+    <t xml:space="preserve">NOTE This field is not currently used when publishing a SPARC dataset. Brief description of the study and the data set. Equivalent to the abstract of a scientific paper. Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
   </si>
   <si>
     <t xml:space="preserve">A really cool dataset that I collected to answer some question.</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">Originating Article DOI</t>
   </si>
   <si>
-    <t xml:space="preserve">DOIs of published articles that contributed to the generation of this dataset</t>
+    <t xml:space="preserve">DOIs of published articles that were generated from this dataset</t>
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.13003/5jchdy</t>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">Metadata Version DO NOT CHANGE</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.1</t>
+    <t xml:space="preserve">1.2.2</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
first pass at dataset description updates for template 2.0
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>TG</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -36,8 +36,6 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
-ID#AAAADMZp7ig
-    (2019-07-01 19:26:26)
 This metadata will be made available to the public as soon as the data set it submitted.
 	-M Martone</t>
         </r>
@@ -48,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t xml:space="preserve">Metadata element</t>
   </si>
@@ -68,10 +66,25 @@
     <t xml:space="preserve">Value 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Additional Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">Value n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metadata Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of this dataset, specifically whether it is experimental or computation. The only valid values are experimental or computational. If experimental subjects are required, if computational, subjects are not required. Set to experimental by default, if you are submitting a computational study be sure to change it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
   </si>
   <si>
     <t xml:space="preserve">Descriptive title for the data set. Equivalent to the title of a scientific paper. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
@@ -89,13 +102,58 @@
     <t xml:space="preserve">Keywords</t>
   </si>
   <si>
-    <t xml:space="preserve">A set of 3-5 keywords other than the above that will aid in search</t>
+    <t xml:space="preserve">A set of keywords to assist in search.</t>
   </si>
   <si>
     <t xml:space="preserve">spinal cord, electrophysiology, RNA-seq, mouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Contributors</t>
+    <t xml:space="preserve">Acknowledgments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acknowledgments beyond funding and contributors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you everyone!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funding sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OT2OD025349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the study purpose for the structured abstract.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study was conducted to demonstrate data wranglers how to fill out dataset templates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study data collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the study data collection process for the structured abstract.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using an earlier version of this template we measured how much it confused data wranglers by counting the number of emails we had to exchange with them in order to fill it out.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study primary conclusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the primary conclusion drawn from the study for the structured abstract.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The primary conclusion of this study is that it is hard to make a good dataset template.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor</t>
   </si>
   <si>
     <t xml:space="preserve">Name of any contributors to the dataset.  These individuals need not have been authors on any publications describing the data, but should be acknowledged for their role in producing and publishing the data set.  If more than one, add each contributor in a new column.</t>
@@ -110,7 +168,7 @@
     <t xml:space="preserve">https://orcid.org/0000-0002-5497-0243</t>
   </si>
   <si>
-    <t xml:space="preserve">Contributor Affiliation</t>
+    <t xml:space="preserve">Contributor affiliation</t>
   </si>
   <si>
     <t xml:space="preserve">Institutional affiliation for contributors</t>
@@ -119,115 +177,115 @@
     <t xml:space="preserve">https://ror.org/0168r3w48</t>
   </si>
   <si>
-    <t xml:space="preserve">Contributor Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contributor role, e.g., PrincipleInvestigator, Creator, CoInvestigator, ContactPerson, DataCollector, DataCurator, DataManager, Distributor, Editor, Producer, ProjectLeader, ProjectManager, ProjectMember, RelatedPerson, Researcher, ResearchGroup, Sponsor, Supervisor, WorkPackageLeader, Other.  These roles are provided by the Data Cite schema.  If more than one, add additional columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Contact Person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes or No if the contributor is a contact person for the dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acknowledgements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acknowledgements beyond funding and contributors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you everyone!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funding sources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OT2OD025349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Originating Article DOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOIs of published articles that were generated from this dataset</t>
+    <t xml:space="preserve">Contributor role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor role. At most one PrincipalInvestigator and at least one CorrespondingAuthor are required. Options are: PrincipalInvestigator, Creator, CoInvestigator, CorrespondingAuthor, DataCollector, DataCurator, DataManager, Distributor, Editor, Producer, ProjectLeader, ProjectManager, ProjectMember, RelatedPerson, Researcher, ResearchGroup, Sponsor, Supervisor, WorkPackageLeader, Other.  These roles are provided by the Data Cite schema.  If more than one, add additional columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataCollector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrincipalInvestigator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CorrespondingAuthor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The identifier for something related to this dataset.</t>
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.13003/5jchdy</t>
   </si>
   <si>
-    <t xml:space="preserve">Protocol URL or DOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URLs (if still private) / DOIs (if public) of protocols from protocols.io related to this dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URLs of additional resources used by this dataset (e.g., a link to a code repository)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/myuser/code-for-really-cool-data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Link Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short description of URL content, you do not need to fill this in for Originating Article DOI or Protocol URL or DOI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">link to GitHub repository for code used in this study</t>
+    <t xml:space="preserve">Related identifier type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of the identifier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relation to related identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relationship that this dataset has to the related identifier. For example the originating article would be this dataset IsDescribedBy originating article.
+The SPARC specific list is:
+HasProtocol
+IsProtocolFor
+UsesSourceCode
+IsSourceCodeUsedBy
+The DataCite list is:
+IsCitedBy,
+Cites,
+IsSupplementTo,
+IsSupplementedBy,
+IsContinuedByContinues,
+IsDescribedBy,
+Describes,
+HasMetadata,
+IsMetadataFor,
+HasVersion,
+IsVersionOf,
+IsNewVersionOf,
+IsPreviousVersionOf,
+IsPartOf,
+HasPart,
+IsPublishedIn,
+IsReferencedBy,
+References,
+IsDocumentedBy,
+Documents,
+IsCompiledBy,
+Compiles,
+IsVariantFormOf,
+IsOriginalFormOf,
+IsIdenticalTo,
+IsReviewedBy,
+Reviews,
+IsDerivedFrom,
+IsSourceOf,
+IsRequiredBy,
+Requires,
+IsObsoletedBy,
+Obsoletes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HasProtocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsDescribedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related identifier description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the referent of the related identifier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The protocol use to generate this dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URLs (if still private) / DOIs (if public) of protocols from protocols.io related to this dataset. This identifier is used to find other datasets that were generated using the same protocol in order to bundle them into a study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The DOI of the published article that describes this dataset or was the primary publication for this dataset.</t>
   </si>
   <si>
     <t xml:space="preserve">Number of subjects</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of unique subjects in this dataset, should match subjects metadata file.</t>
+    <t xml:space="preserve">Number of unique subjects in this dataset, should match subjects metadata file. Only required for experimental datasets.</t>
   </si>
   <si>
     <t xml:space="preserve">Number of samples</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of unique samples in this dataset, should match samples metadata file. Set to zero if there are no samples.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completeness of data set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the data set as uploaded complete or is it part of an ongoing study.  Use "hasNext" to indicate that you expect more data on different subjects as a continuation of this study. Use “hasChildren” to indicate that you expect more data on the same subjects or samples derived from those subjects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasNext, hasChildren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent dataset ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If this is a part of a larger data set, or refereces subjects or samples from a parent dataset, what was the accession number of the prior batch.  You need only give us the number of the last batch, not all batches. If samples and subjects are from multiple parent datasets please create a comma separated list of all parent ids.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N:dataset:c5c2f40f-76be-4979-bfc4-b9f9947231cf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title for complete data set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please give us a provisional title for the entire data set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metadata Version DO NOT CHANGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.3</t>
+    <t xml:space="preserve">Number of unique samples in this dataset, should match samples metadata file. Set to zero if there are no samples. Only required for experimental datasets.</t>
   </si>
 </sst>
 </file>
@@ -236,7 +294,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="9">
@@ -299,7 +357,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,13 +367,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9CC2E5"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FF9CC2E5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA8D08D"/>
-        <bgColor rgb="FF9CC2E5"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -325,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -338,13 +402,6 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -373,7 +430,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,56 +455,76 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -479,7 +556,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFA8D08D"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -488,7 +565,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF1155CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFA8D08D"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -527,26 +604,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="51.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="40.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="7.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="8" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="7.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -573,3162 +648,3221 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="12" t="str">
+      <c r="C6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="21" t="str">
         <f aca="false">HYPERLINK("https://orcid.org/","ORCID ID. If you don't have an ORCID, we suggest you sign up for one.")</f>
         <v>ORCID ID. If you don't have an ORCID, we suggest you sign up for one.</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="10" t="n">
+      <c r="A16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="15" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="10" t="n">
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="15" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="19"/>
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="19"/>
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="19"/>
+      <c r="B24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="19"/>
+      <c r="B25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="19"/>
+      <c r="B26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="19"/>
+      <c r="B27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="19"/>
+      <c r="B28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="19"/>
+      <c r="B29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="19"/>
+      <c r="B30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="19"/>
+      <c r="B31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="19"/>
+      <c r="B32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="19"/>
+      <c r="B33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="19"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="19"/>
+      <c r="B35" s="24"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="19"/>
+      <c r="B36" s="24"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="19"/>
+      <c r="B37" s="24"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="19"/>
+      <c r="B38" s="24"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="19"/>
+      <c r="B39" s="24"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="19"/>
+      <c r="B40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="19"/>
+      <c r="B41" s="24"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="19"/>
+      <c r="B42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="19"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="19"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="19"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="19"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="19"/>
+      <c r="B47" s="24"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="19"/>
+      <c r="B48" s="24"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="19"/>
+      <c r="B49" s="24"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="19"/>
+      <c r="B50" s="24"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="19"/>
+      <c r="B51" s="24"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="19"/>
+      <c r="B52" s="24"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="19"/>
+      <c r="B53" s="24"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="19"/>
+      <c r="B54" s="24"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="19"/>
+      <c r="B55" s="24"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="19"/>
+      <c r="B56" s="24"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="19"/>
+      <c r="B57" s="24"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="19"/>
+      <c r="B58" s="24"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="19"/>
+      <c r="B59" s="24"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="19"/>
+      <c r="B60" s="24"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="19"/>
+      <c r="B61" s="24"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="19"/>
+      <c r="B62" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="19"/>
+      <c r="B63" s="24"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="19"/>
+      <c r="B64" s="24"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="19"/>
+      <c r="B65" s="24"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="19"/>
+      <c r="B66" s="24"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="19"/>
+      <c r="B67" s="24"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="19"/>
+      <c r="B68" s="24"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="19"/>
+      <c r="B69" s="24"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="19"/>
+      <c r="B70" s="24"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="19"/>
+      <c r="B71" s="24"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="19"/>
+      <c r="B72" s="24"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="19"/>
+      <c r="B73" s="24"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="19"/>
+      <c r="B74" s="24"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="19"/>
+      <c r="B75" s="24"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="19"/>
+      <c r="B76" s="24"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="19"/>
+      <c r="B77" s="24"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="19"/>
+      <c r="B78" s="24"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="19"/>
+      <c r="B79" s="24"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="19"/>
+      <c r="B80" s="24"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="19"/>
+      <c r="B81" s="24"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="19"/>
+      <c r="B82" s="24"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="19"/>
+      <c r="B83" s="24"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="19"/>
+      <c r="B84" s="24"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="19"/>
+      <c r="B85" s="24"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="19"/>
+      <c r="B86" s="24"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="19"/>
+      <c r="B87" s="24"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="19"/>
+      <c r="B88" s="24"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="19"/>
+      <c r="B89" s="24"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="19"/>
+      <c r="B90" s="24"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="19"/>
+      <c r="B91" s="24"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="19"/>
+      <c r="B92" s="24"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="19"/>
+      <c r="B93" s="24"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="19"/>
+      <c r="B94" s="24"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="19"/>
+      <c r="B95" s="24"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="19"/>
+      <c r="B96" s="24"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="19"/>
+      <c r="B97" s="24"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="19"/>
+      <c r="B98" s="24"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="19"/>
+      <c r="B99" s="24"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="19"/>
+      <c r="B100" s="24"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="19"/>
+      <c r="B101" s="24"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="19"/>
+      <c r="B102" s="24"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="19"/>
+      <c r="B103" s="24"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="19"/>
+      <c r="B104" s="24"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="19"/>
+      <c r="B105" s="24"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="19"/>
+      <c r="B106" s="24"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="19"/>
+      <c r="B107" s="24"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="19"/>
+      <c r="B108" s="24"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="19"/>
+      <c r="B109" s="24"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="19"/>
+      <c r="B110" s="24"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="19"/>
+      <c r="B111" s="24"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="19"/>
+      <c r="B112" s="24"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="19"/>
+      <c r="B113" s="24"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="19"/>
+      <c r="B114" s="24"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="19"/>
+      <c r="B115" s="24"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="19"/>
+      <c r="B116" s="24"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="19"/>
+      <c r="B117" s="24"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="19"/>
+      <c r="B118" s="24"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="19"/>
+      <c r="B119" s="24"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="19"/>
+      <c r="B120" s="24"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="19"/>
+      <c r="B121" s="24"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="19"/>
+      <c r="B122" s="24"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="19"/>
+      <c r="B123" s="24"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="19"/>
+      <c r="B124" s="24"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="19"/>
+      <c r="B125" s="24"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="19"/>
+      <c r="B126" s="24"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="19"/>
+      <c r="B127" s="24"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="19"/>
+      <c r="B128" s="24"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="19"/>
+      <c r="B129" s="24"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="19"/>
+      <c r="B130" s="24"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="19"/>
+      <c r="B131" s="24"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="19"/>
+      <c r="B132" s="24"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="19"/>
+      <c r="B133" s="24"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="19"/>
+      <c r="B134" s="24"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="19"/>
+      <c r="B135" s="24"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="19"/>
+      <c r="B136" s="24"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="19"/>
+      <c r="B137" s="24"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="19"/>
+      <c r="B138" s="24"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="19"/>
+      <c r="B139" s="24"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="19"/>
+      <c r="B140" s="24"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="19"/>
+      <c r="B141" s="24"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="19"/>
+      <c r="B142" s="24"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="19"/>
+      <c r="B143" s="24"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="19"/>
+      <c r="B144" s="24"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="19"/>
+      <c r="B145" s="24"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="19"/>
+      <c r="B146" s="24"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="19"/>
+      <c r="B147" s="24"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="19"/>
+      <c r="B148" s="24"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="19"/>
+      <c r="B149" s="24"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="19"/>
+      <c r="B150" s="24"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="19"/>
+      <c r="B151" s="24"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="19"/>
+      <c r="B152" s="24"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="19"/>
+      <c r="B153" s="24"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="19"/>
+      <c r="B154" s="24"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="19"/>
+      <c r="B155" s="24"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="19"/>
+      <c r="B156" s="24"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="19"/>
+      <c r="B157" s="24"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="19"/>
+      <c r="B158" s="24"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="19"/>
+      <c r="B159" s="24"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="19"/>
+      <c r="B160" s="24"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="19"/>
+      <c r="B161" s="24"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="19"/>
+      <c r="B162" s="24"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="19"/>
+      <c r="B163" s="24"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="19"/>
+      <c r="B164" s="24"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="19"/>
+      <c r="B165" s="24"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="19"/>
+      <c r="B166" s="24"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="19"/>
+      <c r="B167" s="24"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="19"/>
+      <c r="B168" s="24"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="19"/>
+      <c r="B169" s="24"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="19"/>
+      <c r="B170" s="24"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="19"/>
+      <c r="B171" s="24"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="19"/>
+      <c r="B172" s="24"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="19"/>
+      <c r="B173" s="24"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="19"/>
+      <c r="B174" s="24"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="19"/>
+      <c r="B175" s="24"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="19"/>
+      <c r="B176" s="24"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="19"/>
+      <c r="B177" s="24"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="19"/>
+      <c r="B178" s="24"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="19"/>
+      <c r="B179" s="24"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="19"/>
+      <c r="B180" s="24"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="19"/>
+      <c r="B181" s="24"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="19"/>
+      <c r="B182" s="24"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="19"/>
+      <c r="B183" s="24"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="19"/>
+      <c r="B184" s="24"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="19"/>
+      <c r="B185" s="24"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="19"/>
+      <c r="B186" s="24"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="19"/>
+      <c r="B187" s="24"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="19"/>
+      <c r="B188" s="24"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="19"/>
+      <c r="B189" s="24"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="19"/>
+      <c r="B190" s="24"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="19"/>
+      <c r="B191" s="24"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="19"/>
+      <c r="B192" s="24"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="19"/>
+      <c r="B193" s="24"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="19"/>
+      <c r="B194" s="24"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="19"/>
+      <c r="B195" s="24"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="19"/>
+      <c r="B196" s="24"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="19"/>
+      <c r="B197" s="24"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="19"/>
+      <c r="B198" s="24"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="19"/>
+      <c r="B199" s="24"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="19"/>
+      <c r="B200" s="24"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="19"/>
+      <c r="B201" s="24"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="19"/>
+      <c r="B202" s="24"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="19"/>
+      <c r="B203" s="24"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="19"/>
+      <c r="B204" s="24"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="19"/>
+      <c r="B205" s="24"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="19"/>
+      <c r="B206" s="24"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="19"/>
+      <c r="B207" s="24"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="19"/>
+      <c r="B208" s="24"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="19"/>
+      <c r="B209" s="24"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="19"/>
+      <c r="B210" s="24"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="19"/>
+      <c r="B211" s="24"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="19"/>
+      <c r="B212" s="24"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="19"/>
+      <c r="B213" s="24"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="19"/>
+      <c r="B214" s="24"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="19"/>
+      <c r="B215" s="24"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="19"/>
+      <c r="B216" s="24"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="19"/>
+      <c r="B217" s="24"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="19"/>
+      <c r="B218" s="24"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="19"/>
+      <c r="B219" s="24"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="19"/>
+      <c r="B220" s="24"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="19"/>
+      <c r="B221" s="24"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="19"/>
+      <c r="B222" s="24"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="19"/>
+      <c r="B223" s="24"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="19"/>
+      <c r="B224" s="24"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="19"/>
+      <c r="B225" s="24"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="19"/>
+      <c r="B226" s="24"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="19"/>
+      <c r="B227" s="24"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="19"/>
+      <c r="B228" s="24"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="19"/>
+      <c r="B229" s="24"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="19"/>
+      <c r="B230" s="24"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="19"/>
+      <c r="B231" s="24"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="19"/>
+      <c r="B232" s="24"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="19"/>
+      <c r="B233" s="24"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="19"/>
+      <c r="B234" s="24"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="19"/>
+      <c r="B235" s="24"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="19"/>
+      <c r="B236" s="24"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="19"/>
+      <c r="B237" s="24"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="19"/>
+      <c r="B238" s="24"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="19"/>
+      <c r="B239" s="24"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="19"/>
+      <c r="B240" s="24"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="19"/>
+      <c r="B241" s="24"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="19"/>
+      <c r="B242" s="24"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="19"/>
+      <c r="B243" s="24"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="19"/>
+      <c r="B244" s="24"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="19"/>
+      <c r="B245" s="24"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="19"/>
+      <c r="B246" s="24"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="19"/>
+      <c r="B247" s="24"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="19"/>
+      <c r="B248" s="24"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="19"/>
+      <c r="B249" s="24"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="19"/>
+      <c r="B250" s="24"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="19"/>
+      <c r="B251" s="24"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="19"/>
+      <c r="B252" s="24"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="19"/>
+      <c r="B253" s="24"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="19"/>
+      <c r="B254" s="24"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="19"/>
+      <c r="B255" s="24"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="19"/>
+      <c r="B256" s="24"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="19"/>
+      <c r="B257" s="24"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="19"/>
+      <c r="B258" s="24"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="19"/>
+      <c r="B259" s="24"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="19"/>
+      <c r="B260" s="24"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="19"/>
+      <c r="B261" s="24"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="19"/>
+      <c r="B262" s="24"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="19"/>
+      <c r="B263" s="24"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="19"/>
+      <c r="B264" s="24"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="19"/>
+      <c r="B265" s="24"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="19"/>
+      <c r="B266" s="24"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="19"/>
+      <c r="B267" s="24"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="19"/>
+      <c r="B268" s="24"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="19"/>
+      <c r="B269" s="24"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="19"/>
+      <c r="B270" s="24"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="19"/>
+      <c r="B271" s="24"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="19"/>
+      <c r="B272" s="24"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="19"/>
+      <c r="B273" s="24"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="19"/>
+      <c r="B274" s="24"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="19"/>
+      <c r="B275" s="24"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="19"/>
+      <c r="B276" s="24"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="19"/>
+      <c r="B277" s="24"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="19"/>
+      <c r="B278" s="24"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="19"/>
+      <c r="B279" s="24"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="19"/>
+      <c r="B280" s="24"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="19"/>
+      <c r="B281" s="24"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="19"/>
+      <c r="B282" s="24"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="19"/>
+      <c r="B283" s="24"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="19"/>
+      <c r="B284" s="24"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="19"/>
+      <c r="B285" s="24"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="19"/>
+      <c r="B286" s="24"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="19"/>
+      <c r="B287" s="24"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="19"/>
+      <c r="B288" s="24"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="19"/>
+      <c r="B289" s="24"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="19"/>
+      <c r="B290" s="24"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="19"/>
+      <c r="B291" s="24"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="19"/>
+      <c r="B292" s="24"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="19"/>
+      <c r="B293" s="24"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="19"/>
+      <c r="B294" s="24"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="19"/>
+      <c r="B295" s="24"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="19"/>
+      <c r="B296" s="24"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="19"/>
+      <c r="B297" s="24"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="19"/>
+      <c r="B298" s="24"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="19"/>
+      <c r="B299" s="24"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="19"/>
+      <c r="B300" s="24"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="19"/>
+      <c r="B301" s="24"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="19"/>
+      <c r="B302" s="24"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="19"/>
+      <c r="B303" s="24"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="19"/>
+      <c r="B304" s="24"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="19"/>
+      <c r="B305" s="24"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="19"/>
+      <c r="B306" s="24"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="19"/>
+      <c r="B307" s="24"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="19"/>
+      <c r="B308" s="24"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="19"/>
+      <c r="B309" s="24"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="19"/>
+      <c r="B310" s="24"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="19"/>
+      <c r="B311" s="24"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B312" s="19"/>
+      <c r="B312" s="24"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B313" s="19"/>
+      <c r="B313" s="24"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B314" s="19"/>
+      <c r="B314" s="24"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B315" s="19"/>
+      <c r="B315" s="24"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B316" s="19"/>
+      <c r="B316" s="24"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B317" s="19"/>
+      <c r="B317" s="24"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B318" s="19"/>
+      <c r="B318" s="24"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B319" s="19"/>
+      <c r="B319" s="24"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B320" s="19"/>
+      <c r="B320" s="24"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B321" s="19"/>
+      <c r="B321" s="24"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B322" s="19"/>
+      <c r="B322" s="24"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B323" s="19"/>
+      <c r="B323" s="24"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B324" s="19"/>
+      <c r="B324" s="24"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B325" s="19"/>
+      <c r="B325" s="24"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B326" s="19"/>
+      <c r="B326" s="24"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B327" s="19"/>
+      <c r="B327" s="24"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B328" s="19"/>
+      <c r="B328" s="24"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B329" s="19"/>
+      <c r="B329" s="24"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B330" s="19"/>
+      <c r="B330" s="24"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B331" s="19"/>
+      <c r="B331" s="24"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="19"/>
+      <c r="B332" s="24"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B333" s="19"/>
+      <c r="B333" s="24"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B334" s="19"/>
+      <c r="B334" s="24"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B335" s="19"/>
+      <c r="B335" s="24"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B336" s="19"/>
+      <c r="B336" s="24"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B337" s="19"/>
+      <c r="B337" s="24"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B338" s="19"/>
+      <c r="B338" s="24"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B339" s="19"/>
+      <c r="B339" s="24"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B340" s="19"/>
+      <c r="B340" s="24"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B341" s="19"/>
+      <c r="B341" s="24"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B342" s="19"/>
+      <c r="B342" s="24"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B343" s="19"/>
+      <c r="B343" s="24"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B344" s="19"/>
+      <c r="B344" s="24"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B345" s="19"/>
+      <c r="B345" s="24"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B346" s="19"/>
+      <c r="B346" s="24"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B347" s="19"/>
+      <c r="B347" s="24"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B348" s="19"/>
+      <c r="B348" s="24"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B349" s="19"/>
+      <c r="B349" s="24"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B350" s="19"/>
+      <c r="B350" s="24"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B351" s="19"/>
+      <c r="B351" s="24"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B352" s="19"/>
+      <c r="B352" s="24"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B353" s="19"/>
+      <c r="B353" s="24"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B354" s="19"/>
+      <c r="B354" s="24"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B355" s="19"/>
+      <c r="B355" s="24"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B356" s="19"/>
+      <c r="B356" s="24"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B357" s="19"/>
+      <c r="B357" s="24"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B358" s="19"/>
+      <c r="B358" s="24"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B359" s="19"/>
+      <c r="B359" s="24"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B360" s="19"/>
+      <c r="B360" s="24"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B361" s="19"/>
+      <c r="B361" s="24"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B362" s="19"/>
+      <c r="B362" s="24"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B363" s="19"/>
+      <c r="B363" s="24"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B364" s="19"/>
+      <c r="B364" s="24"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B365" s="19"/>
+      <c r="B365" s="24"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B366" s="19"/>
+      <c r="B366" s="24"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B367" s="19"/>
+      <c r="B367" s="24"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B368" s="19"/>
+      <c r="B368" s="24"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B369" s="19"/>
+      <c r="B369" s="24"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B370" s="19"/>
+      <c r="B370" s="24"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B371" s="19"/>
+      <c r="B371" s="24"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B372" s="19"/>
+      <c r="B372" s="24"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B373" s="19"/>
+      <c r="B373" s="24"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B374" s="19"/>
+      <c r="B374" s="24"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B375" s="19"/>
+      <c r="B375" s="24"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B376" s="19"/>
+      <c r="B376" s="24"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B377" s="19"/>
+      <c r="B377" s="24"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B378" s="19"/>
+      <c r="B378" s="24"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B379" s="19"/>
+      <c r="B379" s="24"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B380" s="19"/>
+      <c r="B380" s="24"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B381" s="19"/>
+      <c r="B381" s="24"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B382" s="19"/>
+      <c r="B382" s="24"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B383" s="19"/>
+      <c r="B383" s="24"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B384" s="19"/>
+      <c r="B384" s="24"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B385" s="19"/>
+      <c r="B385" s="24"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B386" s="19"/>
+      <c r="B386" s="24"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B387" s="19"/>
+      <c r="B387" s="24"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B388" s="19"/>
+      <c r="B388" s="24"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B389" s="19"/>
+      <c r="B389" s="24"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B390" s="19"/>
+      <c r="B390" s="24"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B391" s="19"/>
+      <c r="B391" s="24"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B392" s="19"/>
+      <c r="B392" s="24"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B393" s="19"/>
+      <c r="B393" s="24"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B394" s="19"/>
+      <c r="B394" s="24"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B395" s="19"/>
+      <c r="B395" s="24"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B396" s="19"/>
+      <c r="B396" s="24"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B397" s="19"/>
+      <c r="B397" s="24"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B398" s="19"/>
+      <c r="B398" s="24"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B399" s="19"/>
+      <c r="B399" s="24"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B400" s="19"/>
+      <c r="B400" s="24"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B401" s="19"/>
+      <c r="B401" s="24"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B402" s="19"/>
+      <c r="B402" s="24"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B403" s="19"/>
+      <c r="B403" s="24"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B404" s="19"/>
+      <c r="B404" s="24"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B405" s="19"/>
+      <c r="B405" s="24"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B406" s="19"/>
+      <c r="B406" s="24"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B407" s="19"/>
+      <c r="B407" s="24"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B408" s="19"/>
+      <c r="B408" s="24"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B409" s="19"/>
+      <c r="B409" s="24"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B410" s="19"/>
+      <c r="B410" s="24"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B411" s="19"/>
+      <c r="B411" s="24"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B412" s="19"/>
+      <c r="B412" s="24"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B413" s="19"/>
+      <c r="B413" s="24"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B414" s="19"/>
+      <c r="B414" s="24"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B415" s="19"/>
+      <c r="B415" s="24"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B416" s="19"/>
+      <c r="B416" s="24"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B417" s="19"/>
+      <c r="B417" s="24"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B418" s="19"/>
+      <c r="B418" s="24"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B419" s="19"/>
+      <c r="B419" s="24"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B420" s="19"/>
+      <c r="B420" s="24"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B421" s="19"/>
+      <c r="B421" s="24"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B422" s="19"/>
+      <c r="B422" s="24"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B423" s="19"/>
+      <c r="B423" s="24"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B424" s="19"/>
+      <c r="B424" s="24"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B425" s="19"/>
+      <c r="B425" s="24"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B426" s="19"/>
+      <c r="B426" s="24"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B427" s="19"/>
+      <c r="B427" s="24"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B428" s="19"/>
+      <c r="B428" s="24"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B429" s="19"/>
+      <c r="B429" s="24"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B430" s="19"/>
+      <c r="B430" s="24"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B431" s="19"/>
+      <c r="B431" s="24"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B432" s="19"/>
+      <c r="B432" s="24"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B433" s="19"/>
+      <c r="B433" s="24"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B434" s="19"/>
+      <c r="B434" s="24"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B435" s="19"/>
+      <c r="B435" s="24"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B436" s="19"/>
+      <c r="B436" s="24"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B437" s="19"/>
+      <c r="B437" s="24"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B438" s="19"/>
+      <c r="B438" s="24"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B439" s="19"/>
+      <c r="B439" s="24"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B440" s="19"/>
+      <c r="B440" s="24"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B441" s="19"/>
+      <c r="B441" s="24"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B442" s="19"/>
+      <c r="B442" s="24"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B443" s="19"/>
+      <c r="B443" s="24"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B444" s="19"/>
+      <c r="B444" s="24"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B445" s="19"/>
+      <c r="B445" s="24"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B446" s="19"/>
+      <c r="B446" s="24"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B447" s="19"/>
+      <c r="B447" s="24"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B448" s="19"/>
+      <c r="B448" s="24"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B449" s="19"/>
+      <c r="B449" s="24"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B450" s="19"/>
+      <c r="B450" s="24"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B451" s="19"/>
+      <c r="B451" s="24"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B452" s="19"/>
+      <c r="B452" s="24"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B453" s="19"/>
+      <c r="B453" s="24"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B454" s="19"/>
+      <c r="B454" s="24"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B455" s="19"/>
+      <c r="B455" s="24"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B456" s="19"/>
+      <c r="B456" s="24"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B457" s="19"/>
+      <c r="B457" s="24"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B458" s="19"/>
+      <c r="B458" s="24"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B459" s="19"/>
+      <c r="B459" s="24"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B460" s="19"/>
+      <c r="B460" s="24"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B461" s="19"/>
+      <c r="B461" s="24"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B462" s="19"/>
+      <c r="B462" s="24"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B463" s="19"/>
+      <c r="B463" s="24"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B464" s="19"/>
+      <c r="B464" s="24"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B465" s="19"/>
+      <c r="B465" s="24"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B466" s="19"/>
+      <c r="B466" s="24"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B467" s="19"/>
+      <c r="B467" s="24"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B468" s="19"/>
+      <c r="B468" s="24"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B469" s="19"/>
+      <c r="B469" s="24"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B470" s="19"/>
+      <c r="B470" s="24"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B471" s="19"/>
+      <c r="B471" s="24"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B472" s="19"/>
+      <c r="B472" s="24"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B473" s="19"/>
+      <c r="B473" s="24"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B474" s="19"/>
+      <c r="B474" s="24"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B475" s="19"/>
+      <c r="B475" s="24"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B476" s="19"/>
+      <c r="B476" s="24"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B477" s="19"/>
+      <c r="B477" s="24"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B478" s="19"/>
+      <c r="B478" s="24"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B479" s="19"/>
+      <c r="B479" s="24"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B480" s="19"/>
+      <c r="B480" s="24"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B481" s="19"/>
+      <c r="B481" s="24"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B482" s="19"/>
+      <c r="B482" s="24"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B483" s="19"/>
+      <c r="B483" s="24"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B484" s="19"/>
+      <c r="B484" s="24"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B485" s="19"/>
+      <c r="B485" s="24"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B486" s="19"/>
+      <c r="B486" s="24"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B487" s="19"/>
+      <c r="B487" s="24"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B488" s="19"/>
+      <c r="B488" s="24"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B489" s="19"/>
+      <c r="B489" s="24"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B490" s="19"/>
+      <c r="B490" s="24"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B491" s="19"/>
+      <c r="B491" s="24"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B492" s="19"/>
+      <c r="B492" s="24"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B493" s="19"/>
+      <c r="B493" s="24"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B494" s="19"/>
+      <c r="B494" s="24"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B495" s="19"/>
+      <c r="B495" s="24"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B496" s="19"/>
+      <c r="B496" s="24"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B497" s="19"/>
+      <c r="B497" s="24"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B498" s="19"/>
+      <c r="B498" s="24"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B499" s="19"/>
+      <c r="B499" s="24"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B500" s="19"/>
+      <c r="B500" s="24"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B501" s="19"/>
+      <c r="B501" s="24"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B502" s="19"/>
+      <c r="B502" s="24"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B503" s="19"/>
+      <c r="B503" s="24"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B504" s="19"/>
+      <c r="B504" s="24"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B505" s="19"/>
+      <c r="B505" s="24"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B506" s="19"/>
+      <c r="B506" s="24"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B507" s="19"/>
+      <c r="B507" s="24"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B508" s="19"/>
+      <c r="B508" s="24"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B509" s="19"/>
+      <c r="B509" s="24"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B510" s="19"/>
+      <c r="B510" s="24"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B511" s="19"/>
+      <c r="B511" s="24"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B512" s="19"/>
+      <c r="B512" s="24"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B513" s="19"/>
+      <c r="B513" s="24"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B514" s="19"/>
+      <c r="B514" s="24"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B515" s="19"/>
+      <c r="B515" s="24"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B516" s="19"/>
+      <c r="B516" s="24"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B517" s="19"/>
+      <c r="B517" s="24"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B518" s="19"/>
+      <c r="B518" s="24"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B519" s="19"/>
+      <c r="B519" s="24"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B520" s="19"/>
+      <c r="B520" s="24"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B521" s="19"/>
+      <c r="B521" s="24"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B522" s="19"/>
+      <c r="B522" s="24"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B523" s="19"/>
+      <c r="B523" s="24"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B524" s="19"/>
+      <c r="B524" s="24"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B525" s="19"/>
+      <c r="B525" s="24"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B526" s="19"/>
+      <c r="B526" s="24"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B527" s="19"/>
+      <c r="B527" s="24"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B528" s="19"/>
+      <c r="B528" s="24"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B529" s="19"/>
+      <c r="B529" s="24"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B530" s="19"/>
+      <c r="B530" s="24"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B531" s="19"/>
+      <c r="B531" s="24"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B532" s="19"/>
+      <c r="B532" s="24"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B533" s="19"/>
+      <c r="B533" s="24"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B534" s="19"/>
+      <c r="B534" s="24"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B535" s="19"/>
+      <c r="B535" s="24"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B536" s="19"/>
+      <c r="B536" s="24"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B537" s="19"/>
+      <c r="B537" s="24"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B538" s="19"/>
+      <c r="B538" s="24"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B539" s="19"/>
+      <c r="B539" s="24"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B540" s="19"/>
+      <c r="B540" s="24"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B541" s="19"/>
+      <c r="B541" s="24"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B542" s="19"/>
+      <c r="B542" s="24"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B543" s="19"/>
+      <c r="B543" s="24"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B544" s="19"/>
+      <c r="B544" s="24"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B545" s="19"/>
+      <c r="B545" s="24"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B546" s="19"/>
+      <c r="B546" s="24"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B547" s="19"/>
+      <c r="B547" s="24"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B548" s="19"/>
+      <c r="B548" s="24"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B549" s="19"/>
+      <c r="B549" s="24"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B550" s="19"/>
+      <c r="B550" s="24"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B551" s="19"/>
+      <c r="B551" s="24"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B552" s="19"/>
+      <c r="B552" s="24"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B553" s="19"/>
+      <c r="B553" s="24"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B554" s="19"/>
+      <c r="B554" s="24"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B555" s="19"/>
+      <c r="B555" s="24"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B556" s="19"/>
+      <c r="B556" s="24"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B557" s="19"/>
+      <c r="B557" s="24"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B558" s="19"/>
+      <c r="B558" s="24"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B559" s="19"/>
+      <c r="B559" s="24"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B560" s="19"/>
+      <c r="B560" s="24"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B561" s="19"/>
+      <c r="B561" s="24"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B562" s="19"/>
+      <c r="B562" s="24"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B563" s="19"/>
+      <c r="B563" s="24"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B564" s="19"/>
+      <c r="B564" s="24"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B565" s="19"/>
+      <c r="B565" s="24"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B566" s="19"/>
+      <c r="B566" s="24"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B567" s="19"/>
+      <c r="B567" s="24"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B568" s="19"/>
+      <c r="B568" s="24"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B569" s="19"/>
+      <c r="B569" s="24"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B570" s="19"/>
+      <c r="B570" s="24"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B571" s="19"/>
+      <c r="B571" s="24"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B572" s="19"/>
+      <c r="B572" s="24"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B573" s="19"/>
+      <c r="B573" s="24"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B574" s="19"/>
+      <c r="B574" s="24"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B575" s="19"/>
+      <c r="B575" s="24"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B576" s="19"/>
+      <c r="B576" s="24"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B577" s="19"/>
+      <c r="B577" s="24"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B578" s="19"/>
+      <c r="B578" s="24"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B579" s="19"/>
+      <c r="B579" s="24"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B580" s="19"/>
+      <c r="B580" s="24"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B581" s="19"/>
+      <c r="B581" s="24"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B582" s="19"/>
+      <c r="B582" s="24"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B583" s="19"/>
+      <c r="B583" s="24"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B584" s="19"/>
+      <c r="B584" s="24"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B585" s="19"/>
+      <c r="B585" s="24"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B586" s="19"/>
+      <c r="B586" s="24"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B587" s="19"/>
+      <c r="B587" s="24"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B588" s="19"/>
+      <c r="B588" s="24"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B589" s="19"/>
+      <c r="B589" s="24"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B590" s="19"/>
+      <c r="B590" s="24"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B591" s="19"/>
+      <c r="B591" s="24"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B592" s="19"/>
+      <c r="B592" s="24"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B593" s="19"/>
+      <c r="B593" s="24"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B594" s="19"/>
+      <c r="B594" s="24"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B595" s="19"/>
+      <c r="B595" s="24"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B596" s="19"/>
+      <c r="B596" s="24"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B597" s="19"/>
+      <c r="B597" s="24"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B598" s="19"/>
+      <c r="B598" s="24"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B599" s="19"/>
+      <c r="B599" s="24"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B600" s="19"/>
+      <c r="B600" s="24"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B601" s="19"/>
+      <c r="B601" s="24"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B602" s="19"/>
+      <c r="B602" s="24"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B603" s="19"/>
+      <c r="B603" s="24"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B604" s="19"/>
+      <c r="B604" s="24"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B605" s="19"/>
+      <c r="B605" s="24"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B606" s="19"/>
+      <c r="B606" s="24"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B607" s="19"/>
+      <c r="B607" s="24"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B608" s="19"/>
+      <c r="B608" s="24"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B609" s="19"/>
+      <c r="B609" s="24"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B610" s="19"/>
+      <c r="B610" s="24"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B611" s="19"/>
+      <c r="B611" s="24"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B612" s="19"/>
+      <c r="B612" s="24"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B613" s="19"/>
+      <c r="B613" s="24"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B614" s="19"/>
+      <c r="B614" s="24"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B615" s="19"/>
+      <c r="B615" s="24"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B616" s="19"/>
+      <c r="B616" s="24"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B617" s="19"/>
+      <c r="B617" s="24"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B618" s="19"/>
+      <c r="B618" s="24"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B619" s="19"/>
+      <c r="B619" s="24"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B620" s="19"/>
+      <c r="B620" s="24"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B621" s="19"/>
+      <c r="B621" s="24"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B622" s="19"/>
+      <c r="B622" s="24"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B623" s="19"/>
+      <c r="B623" s="24"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B624" s="19"/>
+      <c r="B624" s="24"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B625" s="19"/>
+      <c r="B625" s="24"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B626" s="19"/>
+      <c r="B626" s="24"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B627" s="19"/>
+      <c r="B627" s="24"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B628" s="19"/>
+      <c r="B628" s="24"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B629" s="19"/>
+      <c r="B629" s="24"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B630" s="19"/>
+      <c r="B630" s="24"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B631" s="19"/>
+      <c r="B631" s="24"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B632" s="19"/>
+      <c r="B632" s="24"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B633" s="19"/>
+      <c r="B633" s="24"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B634" s="19"/>
+      <c r="B634" s="24"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B635" s="19"/>
+      <c r="B635" s="24"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B636" s="19"/>
+      <c r="B636" s="24"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B637" s="19"/>
+      <c r="B637" s="24"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B638" s="19"/>
+      <c r="B638" s="24"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B639" s="19"/>
+      <c r="B639" s="24"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B640" s="19"/>
+      <c r="B640" s="24"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B641" s="19"/>
+      <c r="B641" s="24"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B642" s="19"/>
+      <c r="B642" s="24"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B643" s="19"/>
+      <c r="B643" s="24"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B644" s="19"/>
+      <c r="B644" s="24"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B645" s="19"/>
+      <c r="B645" s="24"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B646" s="19"/>
+      <c r="B646" s="24"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B647" s="19"/>
+      <c r="B647" s="24"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B648" s="19"/>
+      <c r="B648" s="24"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B649" s="19"/>
+      <c r="B649" s="24"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B650" s="19"/>
+      <c r="B650" s="24"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B651" s="19"/>
+      <c r="B651" s="24"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B652" s="19"/>
+      <c r="B652" s="24"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B653" s="19"/>
+      <c r="B653" s="24"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B654" s="19"/>
+      <c r="B654" s="24"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B655" s="19"/>
+      <c r="B655" s="24"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B656" s="19"/>
+      <c r="B656" s="24"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B657" s="19"/>
+      <c r="B657" s="24"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B658" s="19"/>
+      <c r="B658" s="24"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B659" s="19"/>
+      <c r="B659" s="24"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B660" s="19"/>
+      <c r="B660" s="24"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B661" s="19"/>
+      <c r="B661" s="24"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B662" s="19"/>
+      <c r="B662" s="24"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B663" s="19"/>
+      <c r="B663" s="24"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B664" s="19"/>
+      <c r="B664" s="24"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B665" s="19"/>
+      <c r="B665" s="24"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B666" s="19"/>
+      <c r="B666" s="24"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B667" s="19"/>
+      <c r="B667" s="24"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B668" s="19"/>
+      <c r="B668" s="24"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B669" s="19"/>
+      <c r="B669" s="24"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B670" s="19"/>
+      <c r="B670" s="24"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B671" s="19"/>
+      <c r="B671" s="24"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B672" s="19"/>
+      <c r="B672" s="24"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B673" s="19"/>
+      <c r="B673" s="24"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B674" s="19"/>
+      <c r="B674" s="24"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B675" s="19"/>
+      <c r="B675" s="24"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B676" s="19"/>
+      <c r="B676" s="24"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B677" s="19"/>
+      <c r="B677" s="24"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B678" s="19"/>
+      <c r="B678" s="24"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B679" s="19"/>
+      <c r="B679" s="24"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B680" s="19"/>
+      <c r="B680" s="24"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B681" s="19"/>
+      <c r="B681" s="24"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B682" s="19"/>
+      <c r="B682" s="24"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B683" s="19"/>
+      <c r="B683" s="24"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B684" s="19"/>
+      <c r="B684" s="24"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B685" s="19"/>
+      <c r="B685" s="24"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B686" s="19"/>
+      <c r="B686" s="24"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B687" s="19"/>
+      <c r="B687" s="24"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B688" s="19"/>
+      <c r="B688" s="24"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B689" s="19"/>
+      <c r="B689" s="24"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B690" s="19"/>
+      <c r="B690" s="24"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B691" s="19"/>
+      <c r="B691" s="24"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B692" s="19"/>
+      <c r="B692" s="24"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B693" s="19"/>
+      <c r="B693" s="24"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B694" s="19"/>
+      <c r="B694" s="24"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B695" s="19"/>
+      <c r="B695" s="24"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B696" s="19"/>
+      <c r="B696" s="24"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B697" s="19"/>
+      <c r="B697" s="24"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B698" s="19"/>
+      <c r="B698" s="24"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B699" s="19"/>
+      <c r="B699" s="24"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B700" s="19"/>
+      <c r="B700" s="24"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B701" s="19"/>
+      <c r="B701" s="24"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B702" s="19"/>
+      <c r="B702" s="24"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B703" s="19"/>
+      <c r="B703" s="24"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B704" s="19"/>
+      <c r="B704" s="24"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B705" s="19"/>
+      <c r="B705" s="24"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B706" s="19"/>
+      <c r="B706" s="24"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B707" s="19"/>
+      <c r="B707" s="24"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B708" s="19"/>
+      <c r="B708" s="24"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B709" s="19"/>
+      <c r="B709" s="24"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B710" s="19"/>
+      <c r="B710" s="24"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B711" s="19"/>
+      <c r="B711" s="24"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B712" s="19"/>
+      <c r="B712" s="24"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B713" s="19"/>
+      <c r="B713" s="24"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B714" s="19"/>
+      <c r="B714" s="24"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B715" s="19"/>
+      <c r="B715" s="24"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B716" s="19"/>
+      <c r="B716" s="24"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B717" s="19"/>
+      <c r="B717" s="24"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B718" s="19"/>
+      <c r="B718" s="24"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B719" s="19"/>
+      <c r="B719" s="24"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B720" s="19"/>
+      <c r="B720" s="24"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B721" s="19"/>
+      <c r="B721" s="24"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B722" s="19"/>
+      <c r="B722" s="24"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B723" s="19"/>
+      <c r="B723" s="24"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B724" s="19"/>
+      <c r="B724" s="24"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B725" s="19"/>
+      <c r="B725" s="24"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B726" s="19"/>
+      <c r="B726" s="24"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B727" s="19"/>
+      <c r="B727" s="24"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B728" s="19"/>
+      <c r="B728" s="24"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B729" s="19"/>
+      <c r="B729" s="24"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B730" s="19"/>
+      <c r="B730" s="24"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B731" s="19"/>
+      <c r="B731" s="24"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B732" s="19"/>
+      <c r="B732" s="24"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B733" s="19"/>
+      <c r="B733" s="24"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B734" s="19"/>
+      <c r="B734" s="24"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B735" s="19"/>
+      <c r="B735" s="24"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B736" s="19"/>
+      <c r="B736" s="24"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B737" s="19"/>
+      <c r="B737" s="24"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B738" s="19"/>
+      <c r="B738" s="24"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B739" s="19"/>
+      <c r="B739" s="24"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B740" s="19"/>
+      <c r="B740" s="24"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B741" s="19"/>
+      <c r="B741" s="24"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B742" s="19"/>
+      <c r="B742" s="24"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B743" s="19"/>
+      <c r="B743" s="24"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B744" s="19"/>
+      <c r="B744" s="24"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B745" s="19"/>
+      <c r="B745" s="24"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B746" s="19"/>
+      <c r="B746" s="24"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B747" s="19"/>
+      <c r="B747" s="24"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B748" s="19"/>
+      <c r="B748" s="24"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B749" s="19"/>
+      <c r="B749" s="24"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B750" s="19"/>
+      <c r="B750" s="24"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B751" s="19"/>
+      <c r="B751" s="24"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B752" s="19"/>
+      <c r="B752" s="24"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B753" s="19"/>
+      <c r="B753" s="24"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B754" s="19"/>
+      <c r="B754" s="24"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B755" s="19"/>
+      <c r="B755" s="24"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B756" s="19"/>
+      <c r="B756" s="24"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B757" s="19"/>
+      <c r="B757" s="24"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B758" s="19"/>
+      <c r="B758" s="24"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B759" s="19"/>
+      <c r="B759" s="24"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B760" s="19"/>
+      <c r="B760" s="24"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B761" s="19"/>
+      <c r="B761" s="24"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B762" s="19"/>
+      <c r="B762" s="24"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B763" s="19"/>
+      <c r="B763" s="24"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B764" s="19"/>
+      <c r="B764" s="24"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B765" s="19"/>
+      <c r="B765" s="24"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B766" s="19"/>
+      <c r="B766" s="24"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B767" s="19"/>
+      <c r="B767" s="24"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B768" s="19"/>
+      <c r="B768" s="24"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B769" s="19"/>
+      <c r="B769" s="24"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B770" s="19"/>
+      <c r="B770" s="24"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B771" s="19"/>
+      <c r="B771" s="24"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B772" s="19"/>
+      <c r="B772" s="24"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B773" s="19"/>
+      <c r="B773" s="24"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B774" s="19"/>
+      <c r="B774" s="24"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B775" s="19"/>
+      <c r="B775" s="24"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B776" s="19"/>
+      <c r="B776" s="24"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B777" s="19"/>
+      <c r="B777" s="24"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B778" s="19"/>
+      <c r="B778" s="24"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B779" s="19"/>
+      <c r="B779" s="24"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B780" s="19"/>
+      <c r="B780" s="24"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B781" s="19"/>
+      <c r="B781" s="24"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B782" s="19"/>
+      <c r="B782" s="24"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B783" s="19"/>
+      <c r="B783" s="24"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B784" s="19"/>
+      <c r="B784" s="24"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B785" s="19"/>
+      <c r="B785" s="24"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B786" s="19"/>
+      <c r="B786" s="24"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B787" s="19"/>
+      <c r="B787" s="24"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B788" s="19"/>
+      <c r="B788" s="24"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B789" s="19"/>
+      <c r="B789" s="24"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B790" s="19"/>
+      <c r="B790" s="24"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B791" s="19"/>
+      <c r="B791" s="24"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B792" s="19"/>
+      <c r="B792" s="24"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B793" s="19"/>
+      <c r="B793" s="24"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B794" s="19"/>
+      <c r="B794" s="24"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B795" s="19"/>
+      <c r="B795" s="24"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B796" s="19"/>
+      <c r="B796" s="24"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B797" s="19"/>
+      <c r="B797" s="24"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B798" s="19"/>
+      <c r="B798" s="24"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B799" s="19"/>
+      <c r="B799" s="24"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B800" s="19"/>
+      <c r="B800" s="24"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B801" s="19"/>
+      <c r="B801" s="24"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B802" s="19"/>
+      <c r="B802" s="24"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B803" s="19"/>
+      <c r="B803" s="24"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B804" s="19"/>
+      <c r="B804" s="24"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B805" s="19"/>
+      <c r="B805" s="24"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B806" s="19"/>
+      <c r="B806" s="24"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B807" s="19"/>
+      <c r="B807" s="24"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B808" s="19"/>
+      <c r="B808" s="24"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B809" s="19"/>
+      <c r="B809" s="24"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B810" s="19"/>
+      <c r="B810" s="24"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B811" s="19"/>
+      <c r="B811" s="24"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B812" s="19"/>
+      <c r="B812" s="24"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B813" s="19"/>
+      <c r="B813" s="24"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B814" s="19"/>
+      <c r="B814" s="24"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B815" s="19"/>
+      <c r="B815" s="24"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B816" s="19"/>
+      <c r="B816" s="24"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B817" s="19"/>
+      <c r="B817" s="24"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B818" s="19"/>
+      <c r="B818" s="24"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B819" s="19"/>
+      <c r="B819" s="24"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B820" s="19"/>
+      <c r="B820" s="24"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B821" s="19"/>
+      <c r="B821" s="24"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B822" s="19"/>
+      <c r="B822" s="24"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B823" s="19"/>
+      <c r="B823" s="24"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B824" s="19"/>
+      <c r="B824" s="24"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B825" s="19"/>
+      <c r="B825" s="24"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B826" s="19"/>
+      <c r="B826" s="24"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B827" s="19"/>
+      <c r="B827" s="24"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B828" s="19"/>
+      <c r="B828" s="24"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B829" s="19"/>
+      <c r="B829" s="24"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B830" s="19"/>
+      <c r="B830" s="24"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B831" s="19"/>
+      <c r="B831" s="24"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B832" s="19"/>
+      <c r="B832" s="24"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B833" s="19"/>
+      <c r="B833" s="24"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B834" s="19"/>
+      <c r="B834" s="24"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B835" s="19"/>
+      <c r="B835" s="24"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B836" s="19"/>
+      <c r="B836" s="24"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B837" s="19"/>
+      <c r="B837" s="24"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B838" s="19"/>
+      <c r="B838" s="24"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B839" s="19"/>
+      <c r="B839" s="24"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B840" s="19"/>
+      <c r="B840" s="24"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B841" s="19"/>
+      <c r="B841" s="24"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B842" s="19"/>
+      <c r="B842" s="24"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B843" s="19"/>
+      <c r="B843" s="24"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B844" s="19"/>
+      <c r="B844" s="24"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B845" s="19"/>
+      <c r="B845" s="24"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B846" s="19"/>
+      <c r="B846" s="24"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B847" s="19"/>
+      <c r="B847" s="24"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B848" s="19"/>
+      <c r="B848" s="24"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B849" s="19"/>
+      <c r="B849" s="24"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B850" s="19"/>
+      <c r="B850" s="24"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B851" s="19"/>
+      <c r="B851" s="24"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B852" s="19"/>
+      <c r="B852" s="24"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B853" s="19"/>
+      <c r="B853" s="24"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B854" s="19"/>
+      <c r="B854" s="24"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B855" s="19"/>
+      <c r="B855" s="24"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B856" s="19"/>
+      <c r="B856" s="24"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B857" s="19"/>
+      <c r="B857" s="24"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B858" s="19"/>
+      <c r="B858" s="24"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B859" s="19"/>
+      <c r="B859" s="24"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B860" s="19"/>
+      <c r="B860" s="24"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B861" s="19"/>
+      <c r="B861" s="24"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B862" s="19"/>
+      <c r="B862" s="24"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B863" s="19"/>
+      <c r="B863" s="24"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B864" s="19"/>
+      <c r="B864" s="24"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B865" s="19"/>
+      <c r="B865" s="24"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B866" s="19"/>
+      <c r="B866" s="24"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B867" s="19"/>
+      <c r="B867" s="24"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B868" s="19"/>
+      <c r="B868" s="24"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B869" s="19"/>
+      <c r="B869" s="24"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B870" s="19"/>
+      <c r="B870" s="24"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B871" s="19"/>
+      <c r="B871" s="24"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B872" s="19"/>
+      <c r="B872" s="24"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B873" s="19"/>
+      <c r="B873" s="24"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B874" s="19"/>
+      <c r="B874" s="24"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B875" s="19"/>
+      <c r="B875" s="24"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B876" s="19"/>
+      <c r="B876" s="24"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B877" s="19"/>
+      <c r="B877" s="24"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B878" s="19"/>
+      <c r="B878" s="24"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B879" s="19"/>
+      <c r="B879" s="24"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B880" s="19"/>
+      <c r="B880" s="24"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B881" s="19"/>
+      <c r="B881" s="24"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B882" s="19"/>
+      <c r="B882" s="24"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B883" s="19"/>
+      <c r="B883" s="24"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B884" s="19"/>
+      <c r="B884" s="24"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B885" s="19"/>
+      <c r="B885" s="24"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B886" s="19"/>
+      <c r="B886" s="24"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B887" s="19"/>
+      <c r="B887" s="24"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B888" s="19"/>
+      <c r="B888" s="24"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B889" s="19"/>
+      <c r="B889" s="24"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B890" s="19"/>
+      <c r="B890" s="24"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B891" s="19"/>
+      <c r="B891" s="24"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B892" s="19"/>
+      <c r="B892" s="24"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B893" s="19"/>
+      <c r="B893" s="24"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B894" s="19"/>
+      <c r="B894" s="24"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B895" s="19"/>
+      <c r="B895" s="24"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B896" s="19"/>
+      <c r="B896" s="24"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B897" s="19"/>
+      <c r="B897" s="24"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B898" s="19"/>
+      <c r="B898" s="24"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B899" s="19"/>
+      <c r="B899" s="24"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B900" s="19"/>
+      <c r="B900" s="24"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B901" s="19"/>
+      <c r="B901" s="24"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B902" s="19"/>
+      <c r="B902" s="24"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B903" s="19"/>
+      <c r="B903" s="24"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B904" s="19"/>
+      <c r="B904" s="24"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B905" s="19"/>
+      <c r="B905" s="24"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B906" s="19"/>
+      <c r="B906" s="24"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B907" s="19"/>
+      <c r="B907" s="24"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B908" s="19"/>
+      <c r="B908" s="24"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B909" s="19"/>
+      <c r="B909" s="24"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B910" s="19"/>
+      <c r="B910" s="24"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B911" s="19"/>
+      <c r="B911" s="24"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B912" s="19"/>
+      <c r="B912" s="24"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B913" s="19"/>
+      <c r="B913" s="24"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B914" s="19"/>
+      <c r="B914" s="24"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B915" s="19"/>
+      <c r="B915" s="24"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B916" s="19"/>
+      <c r="B916" s="24"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B917" s="19"/>
+      <c r="B917" s="24"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B918" s="19"/>
+      <c r="B918" s="24"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B919" s="19"/>
+      <c r="B919" s="24"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B920" s="19"/>
+      <c r="B920" s="24"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B921" s="19"/>
+      <c r="B921" s="24"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B922" s="19"/>
+      <c r="B922" s="24"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B923" s="19"/>
+      <c r="B923" s="24"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B924" s="19"/>
+      <c r="B924" s="24"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B925" s="19"/>
+      <c r="B925" s="24"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B926" s="19"/>
+      <c r="B926" s="24"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B927" s="19"/>
+      <c r="B927" s="24"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B928" s="19"/>
+      <c r="B928" s="24"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B929" s="19"/>
+      <c r="B929" s="24"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B930" s="19"/>
+      <c r="B930" s="24"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B931" s="19"/>
+      <c r="B931" s="24"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B932" s="19"/>
+      <c r="B932" s="24"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B933" s="19"/>
+      <c r="B933" s="24"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B934" s="19"/>
+      <c r="B934" s="24"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B935" s="19"/>
+      <c r="B935" s="24"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B936" s="19"/>
+      <c r="B936" s="24"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B937" s="19"/>
+      <c r="B937" s="24"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B938" s="19"/>
+      <c r="B938" s="24"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B939" s="19"/>
+      <c r="B939" s="24"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B940" s="19"/>
+      <c r="B940" s="24"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B941" s="19"/>
+      <c r="B941" s="24"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B942" s="19"/>
+      <c r="B942" s="24"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B943" s="19"/>
+      <c r="B943" s="24"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B944" s="19"/>
+      <c r="B944" s="24"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B945" s="19"/>
+      <c r="B945" s="24"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B946" s="19"/>
+      <c r="B946" s="24"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B947" s="19"/>
+      <c r="B947" s="24"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B948" s="19"/>
+      <c r="B948" s="24"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B949" s="19"/>
+      <c r="B949" s="24"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B950" s="19"/>
+      <c r="B950" s="24"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B951" s="19"/>
+      <c r="B951" s="24"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B952" s="19"/>
+      <c r="B952" s="24"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B953" s="19"/>
+      <c r="B953" s="24"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B954" s="19"/>
+      <c r="B954" s="24"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B955" s="19"/>
+      <c r="B955" s="24"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B956" s="19"/>
+      <c r="B956" s="24"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B957" s="19"/>
+      <c r="B957" s="24"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B958" s="19"/>
+      <c r="B958" s="24"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B959" s="19"/>
+      <c r="B959" s="24"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B960" s="19"/>
+      <c r="B960" s="24"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B961" s="19"/>
+      <c r="B961" s="24"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B962" s="19"/>
+      <c r="B962" s="24"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B963" s="19"/>
+      <c r="B963" s="24"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B964" s="19"/>
+      <c r="B964" s="24"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B965" s="19"/>
+      <c r="B965" s="24"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B966" s="19"/>
+      <c r="B966" s="24"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B967" s="19"/>
+      <c r="B967" s="24"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B968" s="19"/>
+      <c r="B968" s="24"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B969" s="19"/>
+      <c r="B969" s="24"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B970" s="19"/>
+      <c r="B970" s="24"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B971" s="19"/>
+      <c r="B971" s="24"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B972" s="19"/>
+      <c r="B972" s="24"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B973" s="19"/>
+      <c r="B973" s="24"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B974" s="19"/>
+      <c r="B974" s="24"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B975" s="19"/>
+      <c r="B975" s="24"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B976" s="19"/>
+      <c r="B976" s="24"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B977" s="19"/>
+      <c r="B977" s="24"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B978" s="19"/>
+      <c r="B978" s="24"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B979" s="19"/>
+      <c r="B979" s="24"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B980" s="19"/>
+      <c r="B980" s="24"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B981" s="19"/>
+      <c r="B981" s="24"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B982" s="19"/>
+      <c r="B982" s="24"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B983" s="19"/>
+      <c r="B983" s="24"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B984" s="19"/>
+      <c r="B984" s="24"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B985" s="19"/>
+      <c r="B985" s="24"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B986" s="19"/>
+      <c r="B986" s="24"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B987" s="19"/>
+      <c r="B987" s="24"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B988" s="19"/>
+      <c r="B988" s="24"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B989" s="19"/>
+      <c r="B989" s="24"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B990" s="19"/>
+      <c r="B990" s="24"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B991" s="19"/>
+      <c r="B991" s="24"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B992" s="19"/>
+      <c r="B992" s="24"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B993" s="19"/>
+      <c r="B993" s="24"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B994" s="19"/>
+      <c r="B994" s="24"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B995" s="19"/>
+      <c r="B995" s="24"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B996" s="19"/>
+      <c r="B996" s="24"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B997" s="19"/>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B997" s="24"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId2" display="https://doi.org/10.13003/5jchdy"/>
-    <hyperlink ref="C14" r:id="rId3" display="https://github.com/myuser/code-for-really-cool-data"/>
+    <hyperlink ref="C16" r:id="rId2" display="https://doi.org/10.13003/5jchdy"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3737,6 +3871,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dataset desc rel ids relation type align to internal
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -215,10 +215,10 @@
   <si>
     <t xml:space="preserve">The relationship that this dataset has to the related identifier. For example the originating article would be this dataset IsDescribedBy originating article.
 The SPARC specific list is:
+IsProtocolFor
 HasProtocol
-IsProtocolFor
-UsesSourceCode
-IsSourceCodeUsedBy
+IsSoftwareFor
+HasSoftware
 The DataCite list is:
 IsCitedBy,
 Cites,
@@ -615,7 +615,7 @@
   <dimension ref="A1:G997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
dataset description file add org techniques and approach
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t xml:space="preserve">Metadata element</t>
   </si>
@@ -162,6 +162,52 @@
     <t xml:space="preserve">The primary conclusion of this study is that it is hard to make a good dataset template.</t>
   </si>
   <si>
+    <t xml:space="preserve">    Study organ system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The major organ systems related to this study.
+autonomic ganglion
+brain
+colon
+heart
+intestine
+kidney
+large intestine
+liver
+lower urinary tract
+lung
+nervous system
+pancreas
+peripheral nervous system
+small intestine
+spinal cord
+spleen
+stomach
+sympathetic nervous system
+urinary bladder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spinal cord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Study approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The experimental approach or approaches taken in this study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electrophysiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Study technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The experimental techniques used in this study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch clamp</t>
+  </si>
+  <si>
     <t xml:space="preserve">    Study collection title</t>
   </si>
   <si>
@@ -201,7 +247,27 @@
     <t xml:space="preserve">    Contributor role</t>
   </si>
   <si>
-    <t xml:space="preserve">Contributor role. At most one PrincipalInvestigator and at least one CorrespondingAuthor are required. Options are: PrincipalInvestigator, Creator, CoInvestigator, CorrespondingAuthor, DataCollector, DataCurator, DataManager, Distributor, Editor, Producer, ProjectLeader, ProjectManager, ProjectMember, RelatedPerson, Researcher, ResearchGroup, Sponsor, Supervisor, WorkPackageLeader, Other.  These roles are provided by the Data Cite schema.  If more than one, add additional columns</t>
+    <t xml:space="preserve">Contributor role. At most one PrincipalInvestigator and at least one CorrespondingAuthor are required. These roles are provided by the Data Cite schema. Options are:
+PrincipalInvestigator
+Creator
+CoInvestigator
+CorrespondingAuthor
+DataCollector
+DataCurator
+DataManager
+Distributor
+Editor
+Producer
+ProjectLeader
+ProjectManager
+ProjectMember
+RelatedPerson
+Researcher
+ResearchGroup
+Sponsor
+Supervisor
+WorkPackageLeader
+Other.</t>
   </si>
   <si>
     <t xml:space="preserve">DataCollector</t>
@@ -673,17 +739,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1002"/>
+  <dimension ref="A1:G1005"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="31.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="7.49"/>
@@ -879,92 +945,86 @@
       <c r="G13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="0"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="B15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="28" t="str">
+      <c r="A17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="0"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="28" t="str">
         <f aca="false">HYPERLINK("https://orcid.org/","ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.")</f>
         <v>ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
@@ -976,108 +1036,138 @@
       <c r="C21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="E22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="1" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>67</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="E24" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="15" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
+      <c r="B25" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
+      <c r="C25" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="15" t="n">
+        <v>75</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="15" t="n">
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="32"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="32"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="32"/>
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="32"/>
@@ -3992,13 +4082,22 @@
     <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1002" s="32"/>
     </row>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1003" s="32"/>
+    </row>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1004" s="32"/>
+    </row>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1005" s="32"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C23" r:id="rId2" display="https://doi.org/10.13003/5jchdy"/>
+    <hyperlink ref="C26" r:id="rId2" display="https://doi.org/10.13003/5jchdy"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
sds 3.0 dataset_description.xlsx update standards section
multiple standards are allowed, compatibility is the responsibility of
the user and standards committees
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">    Consortium data standard</t>
   </si>
   <si>
-    <t xml:space="preserve">The specific consortium data standard that this dataset conforms to. Examples of current know values are SPARC, HEAL-REJOIN, and HEAL-PRECISION.</t>
+    <t xml:space="preserve">The specific consortium data standards that this dataset conforms to. Examples of current know values are SPARC, HEAL, HEAL-REJOIN, and HEAL-PRECISION. List addition standards as separate columns.</t>
   </si>
   <si>
     <t xml:space="preserve">SPARC</t>
@@ -425,7 +425,26 @@
     <t xml:space="preserve">    Identifier type</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of the identifier.</t>
+    <t xml:space="preserve">The type of the identifier. Values:
+ARK
+arXiv
+bibcode
+DOI
+EAN13
+EISSN
+Handle
+IGSN
+ISBN
+ISSN
+ISTC
+LISSN
+LSID
+PMID
+PURL
+UPC
+URL
+URN
+w3id</t>
   </si>
   <si>
     <t xml:space="preserve">DOI</t>
@@ -797,16 +816,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1102,7 +1121,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1196,9 +1215,9 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
@@ -1213,9 +1232,9 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
@@ -1243,13 +1262,13 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="9"/>
@@ -1280,32 +1299,32 @@
       <c r="C11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1336,40 +1355,40 @@
       <c r="G15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>47</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
@@ -1467,7 +1486,7 @@
       <c r="C26" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="20"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -1530,7 +1549,7 @@
       <c r="D31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="18" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1711,7 +1730,7 @@
       <c r="C45" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D45" s="20"/>
+      <c r="D45" s="18"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="s">

</xml_diff>

<commit_message>
template dataset decription bump version to 3.0.1
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -673,12 +673,12 @@
       </c>
       <c r="B2" s="38" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>3.0.1</t>
         </is>
       </c>
       <c r="C2" s="38" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>3.0.1</t>
         </is>
       </c>
       <c r="D2" s="38" t="inlineStr">

</xml_diff>

<commit_message>
template first pass 3.0.2 changes
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/dataset_description.xlsx
+++ b/resources/DatasetTemplate/dataset_description.xlsx
@@ -673,17 +673,17 @@
       </c>
       <c r="B2" s="38" t="inlineStr">
         <is>
-          <t>3.0.1</t>
+          <t>3.0.2</t>
         </is>
       </c>
       <c r="C2" s="38" t="inlineStr">
         <is>
-          <t>3.0.1</t>
+          <t>3.0.2</t>
         </is>
       </c>
       <c r="D2" s="38" t="inlineStr">
         <is>
-          <t>3.0.1</t>
+          <t>3.0.2</t>
         </is>
       </c>
       <c r="E2" s="39" t="n"/>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B31" s="48" t="inlineStr">
         <is>
-          <t>Contributor role. At most one PrincipalInvestigator and at least one CorrespondingAuthor are required. These roles are provided by the Data Cite schema. Options are:
+          <t>Contributor role. At most one PrincipalInvestigator and at least one CorrespondingAuthor are required. Creator cannot be used by itself and requires another role. These roles are provided by the Data Cite schema. Options are:
 PrincipalInvestigator
 Creator
 CoInvestigator

</xml_diff>